<commit_message>
import documents in acquisition to mongo
</commit_message>
<xml_diff>
--- a/app/data/initialdata.xlsx
+++ b/app/data/initialdata.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="1282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1793" uniqueCount="1307">
   <si>
     <t xml:space="preserve">Announcement Date</t>
   </si>
@@ -100,8 +100,7 @@
     <t xml:space="preserve">Allergan Inc</t>
   </si>
   <si>
-    <t xml:space="preserve">AGN
-</t>
+    <t xml:space="preserve">AGN</t>
   </si>
   <si>
     <t xml:space="preserve">California</t>
@@ -273,8 +272,7 @@
     <t xml:space="preserve">Broadcom Corp</t>
   </si>
   <si>
-    <t xml:space="preserve">BRCM
-BDMA</t>
+    <t xml:space="preserve">BRCM</t>
   </si>
   <si>
     <t xml:space="preserve">05/29/15, Reuters, https://www.reuters.com/article/us-broadcom-m-a-avago-correction/avago-to-buy-broadcom-for-37-billion-in-biggest-ever-chip-deal-idUSKBN0OE28220150529</t>
@@ -382,8 +380,7 @@
     <t xml:space="preserve">Guidant Corp</t>
   </si>
   <si>
-    <t xml:space="preserve">GDT
-GDT</t>
+    <t xml:space="preserve">GDT</t>
   </si>
   <si>
     <t xml:space="preserve">Indiana</t>
@@ -825,16 +822,13 @@
     <t xml:space="preserve">Liberty Global Inc</t>
   </si>
   <si>
-    <t xml:space="preserve">LBTYA
-LBTYB
-LBTYK</t>
+    <t xml:space="preserve">LBTYA</t>
   </si>
   <si>
     <t xml:space="preserve">Virgin Media Inc</t>
   </si>
   <si>
-    <t xml:space="preserve">VMED
-VMED</t>
+    <t xml:space="preserve">VMED</t>
   </si>
   <si>
     <t xml:space="preserve">02/05/13;"LexisNexis"; Liberty Global to Acquire Virgin Media Conference Call;https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=bd3cf16d-4def-4e43-b648-0515ab325b7a&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A57PR-D081-DXH2-61NY-00000-00&amp;pddocid=urn%3AcontentItem%3A57PR-D081-DXH2-61NY-00000-00&amp;pdcontentcomponentid=254610&amp;pdteaserkey=sr2&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr2&amp;prid=2706a846-e2ee-4a63-9d48-d7be6c431a3e</t>
@@ -999,8 +993,7 @@
     <t xml:space="preserve">Kerr-McGee Corp</t>
   </si>
   <si>
-    <t xml:space="preserve">KMG
-KMD</t>
+    <t xml:space="preserve">KMG</t>
   </si>
   <si>
     <t xml:space="preserve">Oklahoma</t>
@@ -1069,8 +1062,7 @@
     <t xml:space="preserve">Life Technologies Corp</t>
   </si>
   <si>
-    <t xml:space="preserve">IVN
-IVGN</t>
+    <t xml:space="preserve">IVN</t>
   </si>
   <si>
     <t xml:space="preserve">04/15/13, Reuters, Marc Casper Thermo's CEO punta ad entrare nel mercato del enetic sequencing e, acquistando Life Tech riuscirebbe ad avere la posizione dii seconda azienda più grande ed economica del settore, https://www.reuters.com/article/us-lifetechnologies-thermofisher-idUSBRE93D0A620130415</t>
@@ -3738,6 +3730,9 @@
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=f680fe01-2ab3-4df0-a45e-8e2427187511&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5DMX-GV21-DXH2-62KW-00000-00&amp;pddocid=urn%3AcontentItem%3A5DMX-GV21-DXH2-62KW-00000-00&amp;pdcontentcomponentid=254610&amp;pdteaserkey=sr1&amp;pditab=allpods&amp;ecomp=9fyk&amp;earg=sr1&amp;prid=a2f57cf4-4bce-479b-820a-d4454152ffe3</t>
   </si>
   <si>
+    <t xml:space="preserve">11/17/14;Lexis Nexis</t>
+  </si>
+  <si>
     <t xml:space="preserve">CEO Transcript</t>
   </si>
   <si>
@@ -3753,9 +3748,15 @@
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=52820e4f-0090-4b54-bb9b-a128ae6e3a44&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5J50-Y621-JB72-10K5-00000-00&amp;pddocid=urn%3AcontentItem%3A5J50-Y621-JB72-10K5-00000-00&amp;pdcontentcomponentid=8054&amp;pdteaserkey=sr0&amp;pditab=allpods&amp;ecomp=n7yk&amp;earg=sr0&amp;prid=ea67f203-d1c0-4d83-9b66-97115453b58a</t>
   </si>
   <si>
+    <t xml:space="preserve">02/22/16,"Lexis Nexis" </t>
+  </si>
+  <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=2d0b55ea-d320-413e-addb-e1c77172a418&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5DMP-KDR1-JCMN-Y4RC-00000-00&amp;pddocid=urn%3AcontentItem%3A5DMP-KDR1-JCMN-Y4RC-00000-00&amp;pdcontentcomponentid=299488&amp;pdteaserkey=sr0&amp;pditab=allpods&amp;ecomp=n7yk&amp;earg=sr0&amp;prid=991f52cf-0176-4797-b054-9c4941324bdf</t>
   </si>
   <si>
+    <t xml:space="preserve">11/18/14;"Lexis Nexis",</t>
+  </si>
+  <si>
     <t xml:space="preserve">Analyst Transcript</t>
   </si>
   <si>
@@ -3777,12 +3778,18 @@
     <t xml:space="preserve">https://www.nytimes.com/2009/01/26/business/26drug.html</t>
   </si>
   <si>
+    <t xml:space="preserve">01/26/09, THE NEW YORK TIMES </t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.nature.com/news/2009/090127/full/457520a.html</t>
   </si>
   <si>
     <t xml:space="preserve">https://advance.lexis.com/document/searchwithindocument/?pdmfid=1516831&amp;crid=99137d71-8275-4276-9d60-85eb9f9a753a&amp;pdsearchwithinterm=Wyeth&amp;ecomp=7gc5k&amp;prid=ccf3675e-5088-4844-b214-ca78fb2f4b41</t>
   </si>
   <si>
+    <t xml:space="preserve">04/28/09, Lexis Nexis</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.pfizer.com/news/press-release/press-release-detail/pfizer_and_wyeth_become_one_working_together_for_a_healthier_world</t>
   </si>
   <si>
@@ -3795,15 +3802,21 @@
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=cc326c96-6cad-472d-b641-1212988b891b&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A4VFJ-9R70-TX0H-F1FT-00000-00&amp;pddocid=urn%3AcontentItem%3A4VFJ-9R70-TX0H-F1FT-00000-00&amp;pdcontentcomponentid=288311&amp;pdteaserkey=sr1&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr1&amp;prid=fb910453-46fd-468b-805a-9f5543a83e75</t>
   </si>
   <si>
+    <t xml:space="preserve">01/23/09, Lexis Nexis</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=4fc78464-b46c-4b9b-b1e5-f7e517f3d521&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A4VFK-4RM0-TWX3-K0MY-00000-00&amp;pddocid=urn%3AcontentItem%3A4VFK-4RM0-TWX3-K0MY-00000-00&amp;pdcontentcomponentid=247189&amp;pdteaserkey=sr5&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr5&amp;prid=fb910453-46fd-468b-805a-9f5543a83e75</t>
   </si>
   <si>
-    <t xml:space="preserve">01/24/09, LexisNexis </t>
+    <t xml:space="preserve">01/24/09, Lexis Nexis </t>
   </si>
   <si>
     <t xml:space="preserve">https://www.reuters.com/article/wyeth-pfizer-idUSN2629112920090126.</t>
   </si>
   <si>
+    <t xml:space="preserve">01/26/09, Reuters</t>
+  </si>
+  <si>
     <t xml:space="preserve">Analyst </t>
   </si>
   <si>
@@ -3825,18 +3838,27 @@
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=a99a5e52-72dc-428b-9a27-2ffdad100db6&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5JTS-BWC1-JB20-G1F6-00000-00&amp;pddocid=urn%3AcontentItem%3A5JTS-BWC1-JB20-G1F6-00000-00&amp;pdcontentcomponentid=254610&amp;pdteaserkey=sr0&amp;pditab=allpods&amp;ecomp=y7yk&amp;earg=sr0&amp;prid=c4affc0c-25d5-4615-9e85-267e7de5ab78</t>
   </si>
   <si>
+    <t xml:space="preserve">05/19/16;'Lexis Nexis'</t>
+  </si>
+  <si>
     <t xml:space="preserve">CEO Interview Transcript</t>
   </si>
   <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=ecbe387b-2143-47b2-928d-40834427708f&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5N75-5MK1-DXH2-653R-00000-00&amp;pddocid=urn%3AcontentItem%3A5N75-5MK1-DXH2-653R-00000-00&amp;pdcontentcomponentid=254610&amp;pdteaserkey=sr0&amp;pditab=allpods&amp;ecomp=y7yk&amp;earg=sr0&amp;prid=0d1616fc-0f5a-4cb9-b858-e2090b683321</t>
   </si>
   <si>
+    <t xml:space="preserve">08/09/16;"Lexis Nexis";</t>
+  </si>
+  <si>
     <t xml:space="preserve">Earnings Transcript</t>
   </si>
   <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=f8cc6fc5-3858-4df2-87f8-1b103e88f07a&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5N68-VFM1-DXH2-63VM-00000-00&amp;pddocid=urn%3AcontentItem%3A5N68-VFM1-DXH2-63VM-00000-00&amp;pdcontentcomponentid=254610&amp;pdteaserkey=sr0&amp;pditab=allpods&amp;ecomp=y7yk&amp;earg=sr0&amp;prid=013a0ac6-7016-4d3f-8d12-2b6c9b5b7823</t>
   </si>
   <si>
+    <t xml:space="preserve">02/16/17;"Lexis Nexis"</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://stopthecap.com/2015/05/26/analysis-charter-communications-will-acquire-time-warner-cablebright-house-what-it-means-for-you</t>
   </si>
   <si>
@@ -3867,9 +3889,15 @@
     <t xml:space="preserve">https://advance.lexis.com/api/document?collection=news&amp;id=urn:contentItem:7X1C-YH70-Y8T9-V2MH-00000-00&amp;context=1516831</t>
   </si>
   <si>
+    <t xml:space="preserve">11/04/09; Lexis Nexis</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://advance.lexis.com/api/document?collection=news&amp;id=urn:contentItem:7XV5-N010-Y8Y1-7166-00000-00&amp;context=1516831</t>
   </si>
   <si>
+    <t xml:space="preserve">02/16/10; Lexis Nexis</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.npr.org/templates/story/story.php?storyId=101628010</t>
   </si>
   <si>
@@ -3879,6 +3907,9 @@
     <t xml:space="preserve">https://advance.lexis.com/api/document?collection=news&amp;id=urn:contentItem:7VJF-VMY0-YB00-H1X3-00000-00&amp;context=1516831</t>
   </si>
   <si>
+    <t xml:space="preserve">04/27/09; Lexis Nexis</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://advance.lexis.com/api/document?collection=news&amp;id=urn:contentItem:5149-WPR1-JD35-21CB-00000-00&amp;context=1516831</t>
   </si>
   <si>
@@ -3894,27 +3925,45 @@
     <t xml:space="preserve">https://eu.usatoday.com/story/money/2015/05/28/avago-buying-broadcom/28058329/</t>
   </si>
   <si>
+    <t xml:space="preserve">05/29/15, USA Today</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=1658b80c-9e3d-4c74-8e9a-129471d48814&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5G3M-KNV1-F00X-J00Y-00000-00&amp;pddocid=urn%3AcontentItem%3A5G3M-KNV1-F00X-J00Y-00000-00&amp;pdcontentcomponentid=220623&amp;pdteaserkey=sr1&amp;pditab=allpods&amp;ecomp=wp79k&amp;earg=sr1&amp;prid=04b33bbf-f84d-4fbd-94a3-a34e017c53b3</t>
   </si>
   <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=e56d7697-ce79-4a45-b589-8f95d5fe7895&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5G3D-MYJ1-JBG1-82MR-00000-00&amp;pddocid=urn%3AcontentItem%3A5G3D-MYJ1-JBG1-82MR-00000-00&amp;pdcontentcomponentid=7924&amp;pdteaserkey=sr2&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr2&amp;prid=ebc60f81-be2c-40da-a53c-674384519764</t>
   </si>
   <si>
+    <t xml:space="preserve">05/28/15, Lexis Nexis</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://seekingalpha.com/news/2774896-rbc-upbeat-avago-management-talk-broadcom-deal-track</t>
   </si>
   <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=3b60ece7-41b0-4e71-9572-9cabd5f46c03&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5H9B-6HP1-JBG1-82DY-00000-00&amp;pddocid=urn%3AcontentItem%3A5H9B-6HP1-JBG1-82DY-00000-00&amp;pdcontentcomponentid=7924&amp;pdteaserkey=sr1&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr1&amp;prid=ebc60f81-be2c-40da-a53c-674384519764</t>
   </si>
   <si>
+    <t xml:space="preserve">11/03/15, Lexis Nexis</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=86ea60fb-afa8-44b2-9033-67b1ce2676f3&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5CX1-6W91-DXH2-64RP-00000-00&amp;pddocid=urn%3AcontentItem%3A5CX1-6W91-DXH2-64RP-00000-00&amp;pdcontentcomponentid=254610&amp;pdteaserkey=sr0&amp;pditab=allpods&amp;ecomp=wp79k&amp;earg=sr0&amp;prid=48efe6cf-d94b-44a7-a004-3801e5aac93c</t>
   </si>
   <si>
+    <t xml:space="preserve">08/11/14;"Lexis Nexis"</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=62523afa-9205-4dd7-8ddf-d6577d73a88f&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5C8R-JCP1-JB20-G0M4-00000-00&amp;pddocid=urn%3AcontentItem%3A5C8R-JCP1-JB20-G0M4-00000-00&amp;pdcontentcomponentid=254610&amp;pdteaserkey=sr46&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr46&amp;prid=f4d986f6-37c3-41bd-a634-a31502595b4e</t>
   </si>
   <si>
+    <t xml:space="preserve">05/22/14;"Lexis Nexis"</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=88137753-6dff-40c7-909c-32968a0ec594&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5F62-89J1-F00X-J499-00000-00&amp;pddocid=urn%3AcontentItem%3A5F62-89J1-F00X-J499-00000-00&amp;pdcontentcomponentid=220623&amp;pdteaserkey=sr1&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr1&amp;prid=a25b8e61-24ff-4273-85ce-4a78e10ba6ae</t>
   </si>
   <si>
+    <t xml:space="preserve">01/27/16, "Lexis Nexis"</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=6600cc23-a3e6-4bac-aec1-ce60b130d069&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5HYN-TSW1-JB20-G33B-00000-00&amp;pddocid=urn%3AcontentItem%3A5HYN-TSW1-JB20-G33B-00000-00&amp;pdcontentcomponentid=254610&amp;pdteaserkey=sr9&amp;pditab=allpods&amp;ecomp=wp79k&amp;earg=sr9&amp;prid=d8c2fb8d-1ba8-49c8-bbc4-e1bb40eda9e9</t>
   </si>
   <si>
@@ -3927,24 +3976,36 @@
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=51dd15cd-32ec-4346-90a3-20d6052f98cb&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5CXR-7H61-F03R-N4NM-00000-00&amp;pddocid=urn%3AcontentItem%3A5CXR-7H61-F03R-N4NM-00000-00&amp;pdcontentcomponentid=299488&amp;pdteaserkey=sr6&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr6&amp;prid=b0a45bf2-f061-4aeb-ae28-27c61e714ebd</t>
   </si>
   <si>
+    <t xml:space="preserve">08/17/14;"Lexis Nexis"</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.moodys.com/research/Moodys-rates-post-merger-Kinder-Morgan-Inc-Baa3--PR_313248</t>
   </si>
   <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=9e2f10ee-e8c5-4a2e-96af-463dacee4ab7&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5FKM-5TM1-F03R-N12B-00000-00&amp;pddocid=urn%3AcontentItem%3A5FKM-5TM1-F03R-N12B-00000-00&amp;pdcontentcomponentid=299488&amp;pdteaserkey=sr9&amp;pditab=allpods&amp;ecomp=wp79k&amp;earg=sr9&amp;prid=c930de26-7963-4ad4-ac42-730db605ae2d</t>
   </si>
   <si>
+    <t xml:space="preserve">03/25/15;"Lexis Nexis";</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.reuters.com/article/us-express-scripts-medco-idUSBRE82R0Q720120328</t>
   </si>
   <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=3cc8cd6a-078a-447c-9724-5118b16a0e22&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A53CC-P801-F18Y-Y1P7-00000-00&amp;pddocid=urn%3AcontentItem%3A53CC-P801-F18Y-Y1P7-00000-00&amp;pdcontentcomponentid=8054&amp;pdteaserkey=sr0&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr0&amp;prid=a2117ecb-8b53-497a-842c-43ff0bedccd7exisNexis</t>
   </si>
   <si>
+    <t xml:space="preserve">07/21/11, "Lexis Nexis"</t>
+  </si>
+  <si>
     <t xml:space="preserve">CEO News</t>
   </si>
   <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=41272a57-6e57-4773-93a3-6aed3fa65584&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A54HM-4461-JDTX-7472-00000-00&amp;pddocid=urn%3AcontentItem%3A54HM-4461-JDTX-7472-00000-00&amp;pdcontentcomponentid=8054&amp;pdteaserkey=sr3&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr3&amp;prid=a2117ecb-8b53-497a-842c-43ff0bedccd7</t>
   </si>
   <si>
+    <t xml:space="preserve">12/06/11,"Lexis Nexis"</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.iaatpa.com/images/files/ExpressScriptsMedcoMerger.pdf</t>
   </si>
   <si>
@@ -3954,6 +4015,9 @@
     <t xml:space="preserve">https://www.reuters.com/article/us-expressscripts/express-scripts-to-buy-medco-for-29-billion-idUSTRE76K1GG20110721</t>
   </si>
   <si>
+    <t xml:space="preserve">07/21/11, Reuters</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.nbcnews.com/id/10334047/ns/business-us_business/t/boston-scientific-tops-jj-offer-guidant/#.XRYLovZuJYc</t>
   </si>
   <si>
@@ -3991,6 +4055,9 @@
   </si>
   <si>
     <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=b8a97572-3c10-41ce-8298-bbfaa1f2749f&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A4MRD-7D70-TW8Y-R2TT-00000-00&amp;pddocid=urn%3AcontentItem%3A4MRD-7D70-TW8Y-R2TT-00000-00&amp;pdcontentcomponentid=304481&amp;pdteaserkey=sr4&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr4&amp;prid=93f034c4-e44f-4398-8122-3797bd26523e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01/03/07, Lexis Nexis</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.reuters.com/article/us-caremark-cvs/cvs-ups-caremark-bid-idUSN0824956720070309</t>
@@ -5129,8 +5196,8 @@
   </sheetPr>
   <dimension ref="A1:BC33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15842,13 +15909,13 @@
   <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B64" activeCellId="0" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.85"/>
   </cols>
@@ -15900,10 +15967,10 @@
         <v>1195</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>448</v>
+        <v>1196</v>
       </c>
       <c r="C4" s="58" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -15911,7 +15978,7 @@
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="59" t="s">
-        <v>1197</v>
+        <v>1198</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>477</v>
@@ -15925,7 +15992,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="B6" s="59" t="s">
         <v>480</v>
@@ -15939,7 +16006,7 @@
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>483</v>
@@ -15953,13 +16020,13 @@
     </row>
     <row r="8" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
       <c r="B8" s="148" t="s">
-        <v>494</v>
+        <v>1202</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -15967,13 +16034,13 @@
     </row>
     <row r="9" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1201</v>
+        <v>1203</v>
       </c>
       <c r="B9" s="95" t="s">
-        <v>932</v>
+        <v>1204</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>1202</v>
+        <v>1205</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -15981,13 +16048,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>1203</v>
+        <v>1206</v>
       </c>
       <c r="B10" s="149" t="s">
         <v>939</v>
       </c>
       <c r="C10" s="58" t="s">
-        <v>1204</v>
+        <v>1207</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -15995,13 +16062,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1205</v>
+        <v>1208</v>
       </c>
       <c r="B11" s="149" t="s">
         <v>944</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>1204</v>
+        <v>1207</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -16009,24 +16076,24 @@
     </row>
     <row r="12" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="69" t="s">
-        <v>1206</v>
+        <v>1209</v>
       </c>
       <c r="B12" s="67" t="s">
         <v>951</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>1207</v>
+        <v>1210</v>
       </c>
       <c r="D12" s="69" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="55.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="150" t="s">
-        <v>1208</v>
+        <v>1211</v>
       </c>
       <c r="B13" s="148" t="s">
-        <v>505</v>
+        <v>1212</v>
       </c>
       <c r="C13" s="151" t="s">
         <v>1194</v>
@@ -16037,7 +16104,7 @@
     </row>
     <row r="14" customFormat="false" ht="55.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="59" t="s">
-        <v>1209</v>
+        <v>1213</v>
       </c>
       <c r="B14" s="59" t="s">
         <v>527</v>
@@ -16049,12 +16116,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="176.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="59" t="s">
-        <v>1210</v>
+        <v>1214</v>
       </c>
       <c r="B15" s="150" t="s">
-        <v>534</v>
+        <v>1215</v>
       </c>
       <c r="C15" s="153" t="s">
         <v>1194</v>
@@ -16065,13 +16132,13 @@
     </row>
     <row r="16" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="59" t="s">
-        <v>1211</v>
+        <v>1216</v>
       </c>
       <c r="B16" s="150" t="s">
-        <v>1212</v>
+        <v>1217</v>
       </c>
       <c r="C16" s="153" t="s">
-        <v>1213</v>
+        <v>1218</v>
       </c>
       <c r="D16" s="150" t="n">
         <v>2</v>
@@ -16079,13 +16146,13 @@
     </row>
     <row r="17" s="150" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="59" t="s">
-        <v>1214</v>
+        <v>1219</v>
       </c>
       <c r="B17" s="150" t="s">
-        <v>956</v>
+        <v>1220</v>
       </c>
       <c r="C17" s="153" t="s">
-        <v>1207</v>
+        <v>1210</v>
       </c>
       <c r="D17" s="150" t="n">
         <v>2</v>
@@ -16093,13 +16160,13 @@
     </row>
     <row r="18" s="150" customFormat="true" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="150" t="s">
-        <v>1215</v>
+        <v>1221</v>
       </c>
       <c r="B18" s="150" t="s">
-        <v>1216</v>
+        <v>1222</v>
       </c>
       <c r="C18" s="153" t="s">
-        <v>1207</v>
+        <v>1210</v>
       </c>
       <c r="D18" s="150" t="n">
         <v>2</v>
@@ -16107,13 +16174,13 @@
     </row>
     <row r="19" s="150" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="59" t="s">
-        <v>1217</v>
+        <v>1223</v>
       </c>
       <c r="B19" s="150" t="s">
-        <v>976</v>
+        <v>1224</v>
       </c>
       <c r="C19" s="153" t="s">
-        <v>1218</v>
+        <v>1225</v>
       </c>
       <c r="D19" s="150" t="n">
         <v>2</v>
@@ -16121,13 +16188,13 @@
     </row>
     <row r="20" s="150" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="99" t="s">
-        <v>1219</v>
+        <v>1226</v>
       </c>
       <c r="B20" s="154" t="s">
-        <v>1220</v>
+        <v>1227</v>
       </c>
       <c r="C20" s="155" t="s">
-        <v>1218</v>
+        <v>1225</v>
       </c>
       <c r="D20" s="154" t="n">
         <v>2</v>
@@ -16135,7 +16202,7 @@
     </row>
     <row r="21" s="150" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1221</v>
+        <v>1228</v>
       </c>
       <c r="B21" s="156" t="s">
         <v>546</v>
@@ -16149,7 +16216,7 @@
     </row>
     <row r="22" s="150" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>1222</v>
+        <v>1229</v>
       </c>
       <c r="B22" s="156" t="s">
         <v>559</v>
@@ -16163,27 +16230,27 @@
     </row>
     <row r="23" s="150" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1223</v>
+        <v>1230</v>
       </c>
       <c r="B23" s="156" t="s">
         <v>562</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="24" s="150" customFormat="true" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" s="150" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>1224</v>
+        <v>1231</v>
       </c>
       <c r="B24" s="156" t="s">
-        <v>583</v>
+        <v>1232</v>
       </c>
       <c r="C24" s="58" t="s">
-        <v>1225</v>
+        <v>1233</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>3</v>
@@ -16191,13 +16258,13 @@
     </row>
     <row r="25" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>1226</v>
+        <v>1234</v>
       </c>
       <c r="B25" s="156" t="s">
-        <v>590</v>
+        <v>1235</v>
       </c>
       <c r="C25" s="58" t="s">
-        <v>1227</v>
+        <v>1236</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>3</v>
@@ -16205,13 +16272,13 @@
     </row>
     <row r="26" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1228</v>
+        <v>1237</v>
       </c>
       <c r="B26" s="156" t="s">
-        <v>605</v>
+        <v>1238</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>1227</v>
+        <v>1236</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>3</v>
@@ -16219,13 +16286,13 @@
     </row>
     <row r="27" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="59" t="s">
-        <v>1229</v>
+        <v>1239</v>
       </c>
       <c r="B27" s="95" t="s">
         <v>994</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>1230</v>
+        <v>1240</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>3</v>
@@ -16233,13 +16300,13 @@
     </row>
     <row r="28" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="59" t="s">
-        <v>1231</v>
+        <v>1241</v>
       </c>
       <c r="B28" s="149" t="s">
         <v>1001</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>1230</v>
+        <v>1240</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>3</v>
@@ -16247,13 +16314,13 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="59" t="s">
-        <v>1232</v>
+        <v>1242</v>
       </c>
       <c r="B29" s="149" t="s">
         <v>1006</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>1230</v>
+        <v>1240</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>3</v>
@@ -16261,13 +16328,13 @@
     </row>
     <row r="30" customFormat="false" ht="109.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="59" t="s">
-        <v>1233</v>
+        <v>1243</v>
       </c>
       <c r="B30" s="149" t="s">
         <v>1011</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>1234</v>
+        <v>1244</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>3</v>
@@ -16275,13 +16342,13 @@
     </row>
     <row r="31" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="67" t="s">
-        <v>1235</v>
+        <v>1245</v>
       </c>
       <c r="B31" s="99" t="s">
         <v>1018</v>
       </c>
       <c r="C31" s="66" t="s">
-        <v>1230</v>
+        <v>1240</v>
       </c>
       <c r="D31" s="69" t="n">
         <v>3</v>
@@ -16289,13 +16356,13 @@
     </row>
     <row r="32" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>1236</v>
+        <v>1246</v>
       </c>
       <c r="B32" s="93" t="s">
         <v>622</v>
       </c>
       <c r="C32" s="157" t="s">
-        <v>1213</v>
+        <v>1218</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>4</v>
@@ -16303,7 +16370,7 @@
     </row>
     <row r="33" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="59" t="s">
-        <v>1237</v>
+        <v>1247</v>
       </c>
       <c r="B33" s="95" t="s">
         <v>633</v>
@@ -16317,13 +16384,13 @@
     </row>
     <row r="34" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>1238</v>
+        <v>1248</v>
       </c>
       <c r="B34" s="59" t="s">
-        <v>640</v>
+        <v>1249</v>
       </c>
       <c r="C34" s="58" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>4</v>
@@ -16331,13 +16398,13 @@
     </row>
     <row r="35" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>1239</v>
+        <v>1250</v>
       </c>
       <c r="B35" s="105" t="s">
-        <v>651</v>
+        <v>1251</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>4</v>
@@ -16345,13 +16412,13 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>1240</v>
+        <v>1252</v>
       </c>
       <c r="B36" s="95" t="s">
         <v>1023</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>1241</v>
+        <v>1253</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>4</v>
@@ -16359,13 +16426,13 @@
     </row>
     <row r="37" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>1242</v>
+        <v>1254</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>1028</v>
+        <v>1255</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>1207</v>
+        <v>1210</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>4</v>
@@ -16373,13 +16440,13 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="69" t="s">
-        <v>1243</v>
+        <v>1256</v>
       </c>
       <c r="B38" s="69" t="s">
         <v>1035</v>
       </c>
       <c r="C38" s="66" t="s">
-        <v>1207</v>
+        <v>1210</v>
       </c>
       <c r="D38" s="69" t="n">
         <v>4</v>
@@ -16387,7 +16454,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>1244</v>
+        <v>1257</v>
       </c>
       <c r="B39" s="93" t="s">
         <v>673</v>
@@ -16401,7 +16468,7 @@
     </row>
     <row r="40" customFormat="false" ht="69.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="59" t="s">
-        <v>1245</v>
+        <v>1258</v>
       </c>
       <c r="B40" s="156" t="s">
         <v>676</v>
@@ -16415,24 +16482,24 @@
     </row>
     <row r="41" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>1246</v>
+        <v>1259</v>
       </c>
       <c r="B41" s="93" t="s">
         <v>679</v>
       </c>
       <c r="C41" s="157" t="s">
-        <v>1213</v>
+        <v>1218</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>1247</v>
+        <v>1260</v>
       </c>
       <c r="B42" s="93" t="s">
-        <v>688</v>
+        <v>1261</v>
       </c>
       <c r="C42" s="157" t="s">
         <v>1194</v>
@@ -16443,13 +16510,13 @@
     </row>
     <row r="43" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>1248</v>
+        <v>1262</v>
       </c>
       <c r="B43" s="93" t="s">
         <v>699</v>
       </c>
       <c r="C43" s="157" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>5</v>
@@ -16457,13 +16524,13 @@
     </row>
     <row r="44" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="59" t="s">
-        <v>1249</v>
+        <v>1263</v>
       </c>
       <c r="B44" s="139" t="s">
-        <v>1040</v>
+        <v>1264</v>
       </c>
       <c r="C44" s="157" t="s">
-        <v>1202</v>
+        <v>1205</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>5</v>
@@ -16471,41 +16538,41 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>1250</v>
+        <v>1265</v>
       </c>
       <c r="B45" s="156" t="s">
         <v>1049</v>
       </c>
       <c r="C45" s="157" t="s">
-        <v>1218</v>
+        <v>1225</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="325.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="310.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="154" t="s">
-        <v>1251</v>
+        <v>1266</v>
       </c>
       <c r="B46" s="97" t="s">
-        <v>1052</v>
+        <v>1267</v>
       </c>
       <c r="C46" s="66" t="s">
-        <v>1202</v>
+        <v>1205</v>
       </c>
       <c r="D46" s="69" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>1252</v>
+        <v>1268</v>
       </c>
       <c r="B47" s="59" t="s">
-        <v>720</v>
+        <v>1269</v>
       </c>
       <c r="C47" s="58" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>6</v>
@@ -16513,27 +16580,27 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="150" t="s">
-        <v>1253</v>
+        <v>1270</v>
       </c>
       <c r="B48" s="59" t="s">
-        <v>765</v>
+        <v>1271</v>
       </c>
       <c r="C48" s="58" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>6</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="325.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="310.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="150" t="s">
-        <v>1254</v>
+        <v>1272</v>
       </c>
       <c r="B49" s="59" t="s">
-        <v>794</v>
+        <v>1273</v>
       </c>
       <c r="C49" s="58" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>6</v>
@@ -16541,13 +16608,13 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="59" t="s">
-        <v>1255</v>
+        <v>1274</v>
       </c>
       <c r="B50" s="95" t="s">
-        <v>794</v>
+        <v>1273</v>
       </c>
       <c r="C50" s="58" t="s">
-        <v>1196</v>
+        <v>1197</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>6</v>
@@ -16555,13 +16622,13 @@
     </row>
     <row r="51" customFormat="false" ht="82.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="150" t="s">
-        <v>1256</v>
+        <v>1275</v>
       </c>
       <c r="B51" s="95" t="s">
         <v>1065</v>
       </c>
       <c r="C51" s="58" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>6</v>
@@ -16569,13 +16636,13 @@
     </row>
     <row r="52" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="150" t="s">
-        <v>1258</v>
+        <v>1277</v>
       </c>
       <c r="B52" s="95" t="s">
-        <v>1074</v>
+        <v>1278</v>
       </c>
       <c r="C52" s="58" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>6</v>
@@ -16583,13 +16650,13 @@
     </row>
     <row r="53" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="59" t="s">
-        <v>1259</v>
+        <v>1279</v>
       </c>
       <c r="B53" s="95" t="s">
         <v>1085</v>
       </c>
       <c r="C53" s="58" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D53" s="0" t="n">
         <v>6</v>
@@ -16597,13 +16664,13 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="67" t="s">
-        <v>1260</v>
+        <v>1280</v>
       </c>
       <c r="B54" s="99" t="s">
-        <v>1094</v>
+        <v>1281</v>
       </c>
       <c r="C54" s="66" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D54" s="69" t="n">
         <v>6</v>
@@ -16611,7 +16678,7 @@
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="59" t="s">
-        <v>1261</v>
+        <v>1282</v>
       </c>
       <c r="B55" s="59" t="s">
         <v>831</v>
@@ -16625,13 +16692,13 @@
     </row>
     <row r="56" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="59" t="s">
-        <v>1262</v>
+        <v>1283</v>
       </c>
       <c r="B56" s="59" t="s">
-        <v>840</v>
+        <v>1284</v>
       </c>
       <c r="C56" s="58" t="s">
-        <v>1263</v>
+        <v>1285</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>7</v>
@@ -16639,13 +16706,13 @@
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="59" t="s">
-        <v>1264</v>
+        <v>1286</v>
       </c>
       <c r="B57" s="59" t="s">
-        <v>855</v>
+        <v>1287</v>
       </c>
       <c r="C57" s="58" t="s">
-        <v>1263</v>
+        <v>1285</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>7</v>
@@ -16653,13 +16720,13 @@
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="59" t="s">
-        <v>1265</v>
+        <v>1288</v>
       </c>
       <c r="B58" s="59" t="s">
         <v>860</v>
       </c>
       <c r="C58" s="58" t="s">
-        <v>1263</v>
+        <v>1285</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>7</v>
@@ -16667,13 +16734,13 @@
     </row>
     <row r="59" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="59" t="s">
-        <v>1266</v>
+        <v>1289</v>
       </c>
       <c r="B59" s="59" t="s">
         <v>1105</v>
       </c>
       <c r="C59" s="58" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D59" s="0" t="n">
         <v>7</v>
@@ -16681,13 +16748,13 @@
     </row>
     <row r="60" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="67" t="s">
-        <v>1267</v>
+        <v>1290</v>
       </c>
       <c r="B60" s="99" t="s">
-        <v>1110</v>
+        <v>1291</v>
       </c>
       <c r="C60" s="66" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D60" s="69" t="n">
         <v>7</v>
@@ -16695,13 +16762,13 @@
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="59" t="s">
-        <v>1268</v>
+        <v>1292</v>
       </c>
       <c r="B61" s="59" t="s">
         <v>865</v>
       </c>
       <c r="C61" s="58" t="s">
-        <v>1263</v>
+        <v>1285</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>8</v>
@@ -16709,13 +16776,13 @@
     </row>
     <row r="62" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="59" t="s">
-        <v>1269</v>
+        <v>1293</v>
       </c>
       <c r="B62" s="95" t="s">
         <v>880</v>
       </c>
       <c r="C62" s="58" t="s">
-        <v>1263</v>
+        <v>1285</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>8</v>
@@ -16723,13 +16790,13 @@
     </row>
     <row r="63" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="59" t="s">
-        <v>1270</v>
+        <v>1294</v>
       </c>
       <c r="B63" s="95" t="s">
         <v>885</v>
       </c>
       <c r="C63" s="58" t="s">
-        <v>1263</v>
+        <v>1285</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>8</v>
@@ -16737,13 +16804,13 @@
     </row>
     <row r="64" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="59" t="s">
-        <v>1271</v>
+        <v>1295</v>
       </c>
       <c r="B64" s="95" t="s">
         <v>892</v>
       </c>
       <c r="C64" s="58" t="s">
-        <v>1263</v>
+        <v>1285</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>8</v>
@@ -16751,13 +16818,13 @@
     </row>
     <row r="65" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="59" t="s">
-        <v>1272</v>
+        <v>1296</v>
       </c>
       <c r="B65" s="95" t="s">
         <v>899</v>
       </c>
       <c r="C65" s="58" t="s">
-        <v>1263</v>
+        <v>1285</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>8</v>
@@ -16765,13 +16832,13 @@
     </row>
     <row r="66" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="59" t="s">
-        <v>1273</v>
+        <v>1297</v>
       </c>
       <c r="B66" s="59" t="s">
         <v>1123</v>
       </c>
       <c r="C66" s="58" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>8</v>
@@ -16779,13 +16846,13 @@
     </row>
     <row r="67" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="59" t="s">
-        <v>1274</v>
+        <v>1298</v>
       </c>
       <c r="B67" s="95" t="s">
         <v>1134</v>
       </c>
       <c r="C67" s="58" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D67" s="0" t="n">
         <v>8</v>
@@ -16793,13 +16860,13 @@
     </row>
     <row r="68" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="67" t="s">
-        <v>1275</v>
+        <v>1299</v>
       </c>
       <c r="B68" s="99" t="s">
         <v>1137</v>
       </c>
       <c r="C68" s="66" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D68" s="69" t="n">
         <v>8</v>
@@ -16807,13 +16874,13 @@
     </row>
     <row r="69" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="59" t="s">
-        <v>1276</v>
+        <v>1300</v>
       </c>
       <c r="B69" s="59" t="s">
         <v>910</v>
       </c>
       <c r="C69" s="58" t="s">
-        <v>1263</v>
+        <v>1285</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>9</v>
@@ -16821,13 +16888,13 @@
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="59" t="s">
-        <v>1277</v>
+        <v>1301</v>
       </c>
       <c r="B70" s="59" t="s">
         <v>917</v>
       </c>
       <c r="C70" s="58" t="s">
-        <v>1263</v>
+        <v>1285</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>9</v>
@@ -16835,13 +16902,13 @@
     </row>
     <row r="71" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="59" t="s">
-        <v>1278</v>
+        <v>1302</v>
       </c>
       <c r="B71" s="95" t="s">
         <v>1144</v>
       </c>
       <c r="C71" s="58" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>9</v>
@@ -16849,13 +16916,13 @@
     </row>
     <row r="72" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="59" t="s">
-        <v>1279</v>
+        <v>1303</v>
       </c>
       <c r="B72" s="95" t="s">
         <v>1167</v>
       </c>
       <c r="C72" s="58" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>9</v>
@@ -16863,13 +16930,13 @@
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="59" t="s">
-        <v>1280</v>
+        <v>1304</v>
       </c>
       <c r="B73" s="95" t="s">
-        <v>1174</v>
+        <v>1305</v>
       </c>
       <c r="C73" s="58" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D73" s="0" t="n">
         <v>9</v>
@@ -16877,13 +16944,13 @@
     </row>
     <row r="74" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="67" t="s">
-        <v>1281</v>
+        <v>1306</v>
       </c>
       <c r="B74" s="99" t="s">
         <v>1181</v>
       </c>
       <c r="C74" s="66" t="s">
-        <v>1257</v>
+        <v>1276</v>
       </c>
       <c r="D74" s="69" t="n">
         <v>9</v>

</xml_diff>

<commit_message>
add sentence array as input
</commit_message>
<xml_diff>
--- a/app/data/initialdata.xlsx
+++ b/app/data/initialdata.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2336" uniqueCount="1665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2390" uniqueCount="1683">
   <si>
     <t xml:space="preserve">Announcement Date</t>
   </si>
@@ -4028,27 +4028,6 @@
     <t xml:space="preserve">KMI also intends to sell all of EP's natural gas pipeline assets to KMP and EPB over the next few years</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">10/21/11;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Lexis Nexis</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">cash flow,dividend,debt</t>
   </si>
   <si>
@@ -4061,25 +4040,7 @@
     <t xml:space="preserve">While KMI will be assuming a significant amount of incremental debt as a result of the transaction, the sale of EP's exploration and production business, dropdown transactions to KMP and EPB, and excess cash flows "should allow for a rapid reduction in debt levels."</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">10/21/11, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Lexis Nexis</t>
-    </r>
+    <t xml:space="preserve">10/21/11, Lexis Nexis</t>
   </si>
   <si>
     <t xml:space="preserve">debt,level,ratio,enterprise,EBITDA</t>
@@ -4088,35 +4049,7 @@
     <t xml:space="preserve">KMI expects its ratio of debt to distributions received will be lower than its current level of about 2.5 times by the end of 2013 and that the ratio of consolidated net debt for the entire enterprise (including debt at KMP and EPB) to consolidated EBITDA will return to a little over 4 times by the end of 2014.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">01/09/12;"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Lexis Nexis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">"</t>
-    </r>
+    <t xml:space="preserve">01/09/12;"Lexis Nexis"</t>
   </si>
   <si>
     <t xml:space="preserve">merger,review</t>
@@ -5218,6 +5151,63 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.reuters.com/article/us-caremark-cvs/cvs-ups-caremark-bid-idUSN0824956720070309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.reuters.com/article/us-st-jude-medical-m-a-abbott-idUSKCN0XP1H2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=91162d56-0f58-4ba0-a674-ea4d05ef3b59&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5JNJ-CNW1-JBM5-C1M0-00000-00&amp;pddocid=urn%3AcontentItem%3A5JNJ-CNW1-JBM5-C1M0-00000-00&amp;pdcontentcomponentid=11810&amp;pdteaserkey=sr4&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr4&amp;prid=91bac297-64e3-4074-b689-b84e07ace9dc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.cnbc.com/2018/01/24/abbotts-fourth-quarter-results-2018-profit-forecast-beat-estimates.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=8bfad456-c7c5-415f-b9b7-cedfe328b8ed&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A54PR-8YX1-JDVW-N0TN-00000-00&amp;pddocid=urn%3AcontentItem%3A54PR-8YX1-JDVW-N0TN-00000-00&amp;pdcontentcomponentid=360241&amp;pdteaserkey=sr0&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr0&amp;prid=d342c8f9-655a-4da4-8e14-a468810f0479</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://advance.lexis.com/document?crid=309cdbf2-504d-401a-ad42-eee3dda29a57&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A555J-89V1-DY6W-F446-00000-00&amp;pdcontentcomponentid=160956&amp;pdmfid=1516831&amp;pdisurlapi=true.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=18423f38-9e0d-454f-be92-2e6ec2979574&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5479-67B1-DYRW-V358-00000-00&amp;pddocid=urn%3AcontentItem%3A5479-67B1-DYRW-V358-00000-00&amp;pdcontentcomponentid=7975&amp;pdteaserkey=sr21&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr21&amp;prid=10b9ad1c-22d7-427c-8bcb-b71616cf5ac2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10/21/11;"Lexis Nexis"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://advance.lexis.com/api/document?collection=news&amp;id=urn:contentItem:55R8-MX61-DYG5-701K-00000-00&amp;context=1516831</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=7fa8f696-3334-4e27-9654-36505b94551a&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A57HP-3KJ1-JCMN-Y2TY-00000-00&amp;pddocid=urn%3AcontentItem%3A57HP-3KJ1-JCMN-Y2TY-00000-00&amp;pdcontentcomponentid=299488&amp;pdteaserkey=sr4&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr4&amp;prid=38f05d6c-23bd-49d1-9fc2-383bc70ebdbf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=b6a240fc-722c-4d90-a7f4-2900cce3b0bc&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5NG1-PG31-JCMN-Y494-00000-00&amp;pddocid=urn%3AcontentItem%3A5NG1-PG31-JCMN-Y494-00000-00&amp;pdcontentcomponentid=299488&amp;pdteaserkey=sr14&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr14&amp;prid=35d09642-f154-4146-b9be-40d75cb6ef7c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=cfeea22b-3333-4e42-92e5-97e556b1854d&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5R7W-9D71-F03R-N026-00000-00&amp;pddocid=urn%3AcontentItem%3A5R7W-9D71-F03R-N026-00000-00&amp;pdcontentcomponentid=299488&amp;pdteaserkey=sr11&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr11&amp;prid=35d09642-f154-4146-b9be-40d75cb6ef7c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=a702454e-a8cc-4d71-90c3-3402d5cf729c&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5TT8-TF01-JD33-J40D-00000-00&amp;pddocid=urn%3AcontentItem%3A5TT8-TF01-JD33-J40D-00000-00&amp;pdcontentcomponentid=252475&amp;pdteaserkey=sr0&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr0&amp;prid=38adbeea-fc48-4038-8bba-5dfaac30c561</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.reuters.com/article/us-qwest-centurytel/centurytel-to-buy-qwest-for-10-6-billion-in-stock-idUSTRE63L0ZF20100422</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.nytimes.com/2010/08/05/technology/05qwest.html?searchResultPosition=2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.reuters.com/article/idUSWNA307920120321</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.fool.com/investing/2016/11/23/3-things-investors-need-to-know-about-the-energy-t.aspx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=517a2ebe-1b29-4a9b-b965-24e9a72a47b3&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5MD4-W4R1-JDVW-N151-00000-00&amp;pddocid=urn%3AcontentItem%3A5MD4-W4R1-JDVW-N151-00000-00&amp;pdcontentcomponentid=360317&amp;pdteaserkey=sr17&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr17&amp;prid=749c7706-cfce-400e-8a29-2b13c6bf380f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=d9cbd15c-dab2-45aa-b744-e1ff000ba398&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5MJP-SXP1-JBSN-31TK-00000-00&amp;pddocid=urn%3AcontentItem%3A5MJP-SXP1-JBSN-31TK-00000-00&amp;pdcontentcomponentid=172244&amp;pdteaserkey=sr32&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr32&amp;prid=ba3422a8-9e03-4c6f-baea-57ef84c107b4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://advance.lexis.com/document/?pdmfid=1516831&amp;crid=29661e9f-4ae9-412d-8a97-cd96819f67c8&amp;pddocfullpath=%2Fshared%2Fdocument%2Fnews%2Furn%3AcontentItem%3A5R8Y-64T1-JCMN-Y3H9-00000-00&amp;pddocid=urn%3AcontentItem%3A5R8Y-64T1-JCMN-Y3H9-00000-00&amp;pdcontentcomponentid=299488&amp;pdteaserkey=sr6&amp;pditab=allpods&amp;ecomp=1fyk&amp;earg=sr6&amp;prid=a2b9493b-c4c0-44fd-bda2-9725e0afce30</t>
   </si>
 </sst>
 </file>
@@ -5646,7 +5636,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="166">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6243,10 +6233,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -6257,10 +6243,6 @@
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -6304,6 +6286,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -14849,8 +14843,8 @@
   </sheetPr>
   <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A292" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B75" activeCellId="0" sqref="B75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A170" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B172" activeCellId="0" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18231,13 +18225,13 @@
         <v>11</v>
       </c>
       <c r="B169" s="95" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C169" s="145" t="s">
         <v>1289</v>
       </c>
-      <c r="C169" s="145" t="s">
+      <c r="D169" s="59" t="s">
         <v>1290</v>
-      </c>
-      <c r="D169" s="59" t="s">
-        <v>1291</v>
       </c>
       <c r="E169" s="119" t="n">
         <v>-1</v>
@@ -18251,13 +18245,13 @@
         <v>11</v>
       </c>
       <c r="B170" s="95" t="s">
-        <v>1289</v>
+        <v>1262</v>
       </c>
       <c r="C170" s="145" t="s">
+        <v>1291</v>
+      </c>
+      <c r="D170" s="59" t="s">
         <v>1292</v>
-      </c>
-      <c r="D170" s="59" t="s">
-        <v>1293</v>
       </c>
       <c r="E170" s="119" t="n">
         <v>0</v>
@@ -18271,14 +18265,14 @@
         <v>11</v>
       </c>
       <c r="B171" s="84" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C171" s="147" t="s">
         <v>1294</v>
       </c>
-      <c r="C171" s="147" t="s">
+      <c r="D171" s="103" t="s">
         <v>1295</v>
       </c>
-      <c r="D171" s="103" t="s">
-        <v>1296</v>
-      </c>
       <c r="E171" s="84" t="n">
         <v>1</v>
       </c>
@@ -18286,18 +18280,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="172" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="58" t="n">
         <v>11</v>
       </c>
       <c r="B172" s="95" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C172" s="145" t="s">
         <v>1297</v>
       </c>
-      <c r="C172" s="145" t="s">
+      <c r="D172" s="59" t="s">
         <v>1298</v>
-      </c>
-      <c r="D172" s="59" t="s">
-        <v>1299</v>
       </c>
       <c r="E172" s="119" t="n">
         <v>1</v>
@@ -18311,13 +18305,13 @@
         <v>11</v>
       </c>
       <c r="B173" s="95" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="C173" s="145" t="s">
+        <v>1299</v>
+      </c>
+      <c r="D173" s="59" t="s">
         <v>1300</v>
-      </c>
-      <c r="D173" s="59" t="s">
-        <v>1301</v>
       </c>
       <c r="E173" s="119" t="n">
         <v>-1</v>
@@ -18331,13 +18325,13 @@
         <v>11</v>
       </c>
       <c r="B174" s="95" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="C174" s="145" t="s">
+        <v>1301</v>
+      </c>
+      <c r="D174" s="59" t="s">
         <v>1302</v>
-      </c>
-      <c r="D174" s="59" t="s">
-        <v>1303</v>
       </c>
       <c r="E174" s="119" t="n">
         <v>0</v>
@@ -18351,13 +18345,13 @@
         <v>11</v>
       </c>
       <c r="B175" s="95" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="C175" s="145" t="s">
+        <v>1303</v>
+      </c>
+      <c r="D175" s="59" t="s">
         <v>1304</v>
-      </c>
-      <c r="D175" s="59" t="s">
-        <v>1305</v>
       </c>
       <c r="E175" s="119" t="n">
         <v>-1</v>
@@ -18371,13 +18365,13 @@
         <v>11</v>
       </c>
       <c r="B176" s="95" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="C176" s="145" t="s">
+        <v>1305</v>
+      </c>
+      <c r="D176" s="59" t="s">
         <v>1306</v>
-      </c>
-      <c r="D176" s="59" t="s">
-        <v>1307</v>
       </c>
       <c r="E176" s="119" t="n">
         <v>-1</v>
@@ -18391,13 +18385,13 @@
         <v>11</v>
       </c>
       <c r="B177" s="84" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="C177" s="147" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D177" s="103" t="s">
         <v>1308</v>
-      </c>
-      <c r="D177" s="103" t="s">
-        <v>1309</v>
       </c>
       <c r="E177" s="84" t="n">
         <v>0</v>
@@ -18411,13 +18405,13 @@
         <v>11</v>
       </c>
       <c r="B178" s="95" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C178" s="145" t="s">
         <v>1310</v>
       </c>
-      <c r="C178" s="145" t="s">
+      <c r="D178" s="59" t="s">
         <v>1311</v>
-      </c>
-      <c r="D178" s="59" t="s">
-        <v>1312</v>
       </c>
       <c r="E178" s="119" t="n">
         <v>1</v>
@@ -18431,13 +18425,13 @@
         <v>11</v>
       </c>
       <c r="B179" s="95" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C179" s="145" t="s">
+        <v>1312</v>
+      </c>
+      <c r="D179" s="59" t="s">
         <v>1313</v>
-      </c>
-      <c r="D179" s="59" t="s">
-        <v>1314</v>
       </c>
       <c r="E179" s="119" t="n">
         <v>1</v>
@@ -18451,13 +18445,13 @@
         <v>11</v>
       </c>
       <c r="B180" s="95" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C180" s="145" t="s">
+        <v>1314</v>
+      </c>
+      <c r="D180" s="59" t="s">
         <v>1315</v>
-      </c>
-      <c r="D180" s="59" t="s">
-        <v>1316</v>
       </c>
       <c r="E180" s="119" t="n">
         <v>0</v>
@@ -18471,13 +18465,13 @@
         <v>11</v>
       </c>
       <c r="B181" s="95" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C181" s="145" t="s">
+        <v>1316</v>
+      </c>
+      <c r="D181" s="59" t="s">
         <v>1317</v>
-      </c>
-      <c r="D181" s="59" t="s">
-        <v>1318</v>
       </c>
       <c r="E181" s="119" t="n">
         <v>0</v>
@@ -18491,13 +18485,13 @@
         <v>11</v>
       </c>
       <c r="B182" s="95" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C182" s="145" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D182" s="59" t="s">
         <v>1319</v>
-      </c>
-      <c r="D182" s="59" t="s">
-        <v>1320</v>
       </c>
       <c r="E182" s="119" t="n">
         <v>1</v>
@@ -18511,13 +18505,13 @@
         <v>11</v>
       </c>
       <c r="B183" s="95" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C183" s="145" t="s">
+        <v>1320</v>
+      </c>
+      <c r="D183" s="59" t="s">
         <v>1321</v>
-      </c>
-      <c r="D183" s="59" t="s">
-        <v>1322</v>
       </c>
       <c r="E183" s="119" t="n">
         <v>-1</v>
@@ -18531,13 +18525,13 @@
         <v>11</v>
       </c>
       <c r="B184" s="84" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C184" s="147" t="s">
+        <v>1322</v>
+      </c>
+      <c r="D184" s="103" t="s">
         <v>1323</v>
-      </c>
-      <c r="D184" s="103" t="s">
-        <v>1324</v>
       </c>
       <c r="E184" s="84" t="n">
         <v>0</v>
@@ -18551,13 +18545,13 @@
         <v>11</v>
       </c>
       <c r="B185" s="95" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C185" s="145" t="s">
         <v>1325</v>
       </c>
-      <c r="C185" s="145" t="s">
+      <c r="D185" s="59" t="s">
         <v>1326</v>
-      </c>
-      <c r="D185" s="59" t="s">
-        <v>1327</v>
       </c>
       <c r="E185" s="119" t="n">
         <v>1</v>
@@ -18571,13 +18565,13 @@
         <v>11</v>
       </c>
       <c r="B186" s="95" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="C186" s="145" t="s">
+        <v>1327</v>
+      </c>
+      <c r="D186" s="59" t="s">
         <v>1328</v>
-      </c>
-      <c r="D186" s="59" t="s">
-        <v>1329</v>
       </c>
       <c r="E186" s="119" t="n">
         <v>1</v>
@@ -18591,13 +18585,13 @@
         <v>11</v>
       </c>
       <c r="B187" s="95" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="C187" s="145" t="s">
+        <v>1329</v>
+      </c>
+      <c r="D187" s="59" t="s">
         <v>1330</v>
-      </c>
-      <c r="D187" s="59" t="s">
-        <v>1331</v>
       </c>
       <c r="E187" s="119" t="n">
         <v>0</v>
@@ -18611,13 +18605,13 @@
         <v>11</v>
       </c>
       <c r="B188" s="95" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="C188" s="145" t="s">
+        <v>1331</v>
+      </c>
+      <c r="D188" s="59" t="s">
         <v>1332</v>
-      </c>
-      <c r="D188" s="59" t="s">
-        <v>1333</v>
       </c>
       <c r="E188" s="119" t="n">
         <v>1</v>
@@ -18631,13 +18625,13 @@
         <v>11</v>
       </c>
       <c r="B189" s="84" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="C189" s="147" t="s">
+        <v>1333</v>
+      </c>
+      <c r="D189" s="103" t="s">
         <v>1334</v>
-      </c>
-      <c r="D189" s="103" t="s">
-        <v>1335</v>
       </c>
       <c r="E189" s="84" t="n">
         <v>1</v>
@@ -18651,13 +18645,13 @@
         <v>11</v>
       </c>
       <c r="B190" s="95" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C190" s="146" t="s">
         <v>1336</v>
       </c>
-      <c r="C190" s="146" t="s">
+      <c r="D190" s="59" t="s">
         <v>1337</v>
-      </c>
-      <c r="D190" s="59" t="s">
-        <v>1338</v>
       </c>
       <c r="E190" s="119" t="n">
         <v>-1</v>
@@ -18671,13 +18665,13 @@
         <v>11</v>
       </c>
       <c r="B191" s="95" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C191" s="145" t="s">
+        <v>1338</v>
+      </c>
+      <c r="D191" s="59" t="s">
         <v>1339</v>
-      </c>
-      <c r="D191" s="59" t="s">
-        <v>1340</v>
       </c>
       <c r="E191" s="119" t="n">
         <v>1</v>
@@ -18691,13 +18685,13 @@
         <v>11</v>
       </c>
       <c r="B192" s="95" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C192" s="145" t="s">
+        <v>1340</v>
+      </c>
+      <c r="D192" s="59" t="s">
         <v>1341</v>
-      </c>
-      <c r="D192" s="59" t="s">
-        <v>1342</v>
       </c>
       <c r="E192" s="119" t="n">
         <v>0</v>
@@ -18711,13 +18705,13 @@
         <v>11</v>
       </c>
       <c r="B193" s="95" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C193" s="145" t="s">
+        <v>1342</v>
+      </c>
+      <c r="D193" s="59" t="s">
         <v>1343</v>
-      </c>
-      <c r="D193" s="59" t="s">
-        <v>1344</v>
       </c>
       <c r="E193" s="119" t="n">
         <v>1</v>
@@ -18731,13 +18725,13 @@
         <v>11</v>
       </c>
       <c r="B194" s="95" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C194" s="145" t="s">
+        <v>1344</v>
+      </c>
+      <c r="D194" s="59" t="s">
         <v>1345</v>
-      </c>
-      <c r="D194" s="59" t="s">
-        <v>1346</v>
       </c>
       <c r="E194" s="119" t="n">
         <v>-1</v>
@@ -18751,13 +18745,13 @@
         <v>11</v>
       </c>
       <c r="B195" s="95" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C195" s="145" t="s">
+        <v>1346</v>
+      </c>
+      <c r="D195" s="59" t="s">
         <v>1347</v>
-      </c>
-      <c r="D195" s="59" t="s">
-        <v>1348</v>
       </c>
       <c r="E195" s="119" t="n">
         <v>1</v>
@@ -18771,13 +18765,13 @@
         <v>11</v>
       </c>
       <c r="B196" s="95" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C196" s="145" t="s">
+        <v>1348</v>
+      </c>
+      <c r="D196" s="59" t="s">
         <v>1349</v>
-      </c>
-      <c r="D196" s="59" t="s">
-        <v>1350</v>
       </c>
       <c r="E196" s="119" t="n">
         <v>0</v>
@@ -18791,13 +18785,13 @@
         <v>11</v>
       </c>
       <c r="B197" s="95" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C197" s="145" t="s">
+        <v>1350</v>
+      </c>
+      <c r="D197" s="59" t="s">
         <v>1351</v>
-      </c>
-      <c r="D197" s="59" t="s">
-        <v>1352</v>
       </c>
       <c r="E197" s="119" t="n">
         <v>1</v>
@@ -18811,13 +18805,13 @@
         <v>11</v>
       </c>
       <c r="B198" s="95" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C198" s="145" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D198" s="59" t="s">
         <v>1353</v>
-      </c>
-      <c r="D198" s="59" t="s">
-        <v>1354</v>
       </c>
       <c r="E198" s="119" t="n">
         <v>0</v>
@@ -18831,13 +18825,13 @@
         <v>11</v>
       </c>
       <c r="B199" s="69" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
       <c r="C199" s="148" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D199" s="67" t="s">
         <v>1355</v>
-      </c>
-      <c r="D199" s="67" t="s">
-        <v>1356</v>
       </c>
       <c r="E199" s="69" t="n">
         <v>-1</v>
@@ -18851,13 +18845,13 @@
         <v>12</v>
       </c>
       <c r="B200" s="95" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C200" s="146" t="s">
         <v>1357</v>
       </c>
-      <c r="C200" s="146" t="s">
+      <c r="D200" s="146" t="s">
         <v>1358</v>
-      </c>
-      <c r="D200" s="146" t="s">
-        <v>1359</v>
       </c>
       <c r="E200" s="119" t="n">
         <v>0</v>
@@ -18871,13 +18865,13 @@
         <v>12</v>
       </c>
       <c r="B201" s="95" t="s">
-        <v>1357</v>
+        <v>1356</v>
       </c>
       <c r="C201" s="146" t="s">
+        <v>1359</v>
+      </c>
+      <c r="D201" s="146" t="s">
         <v>1360</v>
-      </c>
-      <c r="D201" s="146" t="s">
-        <v>1361</v>
       </c>
       <c r="E201" s="119" t="n">
         <v>0</v>
@@ -18891,13 +18885,13 @@
         <v>12</v>
       </c>
       <c r="B202" s="95" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C202" s="146" t="s">
         <v>1362</v>
       </c>
-      <c r="C202" s="146" t="s">
+      <c r="D202" s="146" t="s">
         <v>1363</v>
-      </c>
-      <c r="D202" s="146" t="s">
-        <v>1364</v>
       </c>
       <c r="E202" s="119" t="n">
         <v>0</v>
@@ -18911,13 +18905,13 @@
         <v>12</v>
       </c>
       <c r="B203" s="95" t="s">
-        <v>1362</v>
+        <v>1361</v>
       </c>
       <c r="C203" s="146" t="s">
-        <v>1358</v>
+        <v>1357</v>
       </c>
       <c r="D203" s="146" t="s">
-        <v>1365</v>
+        <v>1364</v>
       </c>
       <c r="E203" s="119" t="n">
         <v>0</v>
@@ -18931,13 +18925,13 @@
         <v>12</v>
       </c>
       <c r="B204" s="95" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C204" s="146" t="s">
         <v>1366</v>
       </c>
-      <c r="C204" s="146" t="s">
+      <c r="D204" s="146" t="s">
         <v>1367</v>
-      </c>
-      <c r="D204" s="146" t="s">
-        <v>1368</v>
       </c>
       <c r="E204" s="119" t="n">
         <v>1</v>
@@ -18951,13 +18945,13 @@
         <v>12</v>
       </c>
       <c r="B205" s="95" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C205" s="146" t="s">
+        <v>1368</v>
+      </c>
+      <c r="D205" s="146" t="s">
         <v>1369</v>
-      </c>
-      <c r="D205" s="146" t="s">
-        <v>1370</v>
       </c>
       <c r="E205" s="119" t="n">
         <v>0</v>
@@ -18971,13 +18965,13 @@
         <v>12</v>
       </c>
       <c r="B206" s="95" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C206" s="146" t="s">
+        <v>1370</v>
+      </c>
+      <c r="D206" s="146" t="s">
         <v>1371</v>
-      </c>
-      <c r="D206" s="146" t="s">
-        <v>1372</v>
       </c>
       <c r="E206" s="119" t="n">
         <v>1</v>
@@ -18991,13 +18985,13 @@
         <v>12</v>
       </c>
       <c r="B207" s="95" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C207" s="146" t="s">
+        <v>1372</v>
+      </c>
+      <c r="D207" s="146" t="s">
         <v>1373</v>
-      </c>
-      <c r="D207" s="146" t="s">
-        <v>1374</v>
       </c>
       <c r="E207" s="119" t="n">
         <v>0</v>
@@ -19011,13 +19005,13 @@
         <v>12</v>
       </c>
       <c r="B208" s="95" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C208" s="146" t="s">
+        <v>1374</v>
+      </c>
+      <c r="D208" s="146" t="s">
         <v>1375</v>
-      </c>
-      <c r="D208" s="146" t="s">
-        <v>1376</v>
       </c>
       <c r="E208" s="119" t="n">
         <v>0</v>
@@ -19031,13 +19025,13 @@
         <v>12</v>
       </c>
       <c r="B209" s="95" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C209" s="146" t="s">
+        <v>1376</v>
+      </c>
+      <c r="D209" s="146" t="s">
         <v>1377</v>
-      </c>
-      <c r="D209" s="146" t="s">
-        <v>1378</v>
       </c>
       <c r="E209" s="119" t="n">
         <v>0</v>
@@ -19051,13 +19045,13 @@
         <v>12</v>
       </c>
       <c r="B210" s="95" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C210" s="146" t="s">
+        <v>1378</v>
+      </c>
+      <c r="D210" s="146" t="s">
         <v>1379</v>
-      </c>
-      <c r="D210" s="146" t="s">
-        <v>1380</v>
       </c>
       <c r="E210" s="119" t="n">
         <v>0</v>
@@ -19071,13 +19065,13 @@
         <v>12</v>
       </c>
       <c r="B211" s="95" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C211" s="146" t="s">
+        <v>1380</v>
+      </c>
+      <c r="D211" s="146" t="s">
         <v>1381</v>
-      </c>
-      <c r="D211" s="146" t="s">
-        <v>1382</v>
       </c>
       <c r="E211" s="119" t="n">
         <v>0</v>
@@ -19091,13 +19085,13 @@
         <v>12</v>
       </c>
       <c r="B212" s="84" t="s">
-        <v>1366</v>
+        <v>1365</v>
       </c>
       <c r="C212" s="147" t="s">
+        <v>1382</v>
+      </c>
+      <c r="D212" s="147" t="s">
         <v>1383</v>
-      </c>
-      <c r="D212" s="147" t="s">
-        <v>1384</v>
       </c>
       <c r="E212" s="84" t="n">
         <v>0</v>
@@ -19111,18 +19105,18 @@
         <v>13</v>
       </c>
       <c r="B213" s="95" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C213" s="146" t="s">
         <v>1385</v>
       </c>
-      <c r="C213" s="146" t="s">
+      <c r="D213" s="146" t="s">
         <v>1386</v>
-      </c>
-      <c r="D213" s="146" t="s">
-        <v>1387</v>
       </c>
       <c r="E213" s="119" t="n">
         <v>0</v>
       </c>
-      <c r="F213" s="149" t="n">
+      <c r="F213" s="57" t="n">
         <v>0</v>
       </c>
     </row>
@@ -19131,18 +19125,18 @@
         <v>13</v>
       </c>
       <c r="B214" s="95" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="C214" s="146" t="s">
+        <v>1387</v>
+      </c>
+      <c r="D214" s="146" t="s">
         <v>1388</v>
-      </c>
-      <c r="D214" s="146" t="s">
-        <v>1389</v>
       </c>
       <c r="E214" s="119" t="n">
         <v>0</v>
       </c>
-      <c r="F214" s="149" t="n">
+      <c r="F214" s="57" t="n">
         <v>0</v>
       </c>
     </row>
@@ -19151,13 +19145,13 @@
         <v>13</v>
       </c>
       <c r="B215" s="95" t="s">
-        <v>1385</v>
+        <v>1384</v>
       </c>
       <c r="C215" s="148" t="s">
+        <v>1389</v>
+      </c>
+      <c r="D215" s="148" t="s">
         <v>1390</v>
-      </c>
-      <c r="D215" s="148" t="s">
-        <v>1391</v>
       </c>
       <c r="E215" s="69" t="n">
         <v>0</v>
@@ -19171,13 +19165,13 @@
         <v>14</v>
       </c>
       <c r="B216" s="139" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C216" s="59" t="s">
         <v>1392</v>
       </c>
-      <c r="C216" s="59" t="s">
+      <c r="D216" s="59" t="s">
         <v>1393</v>
-      </c>
-      <c r="D216" s="59" t="s">
-        <v>1394</v>
       </c>
       <c r="E216" s="119" t="n">
         <v>0</v>
@@ -19191,13 +19185,13 @@
         <v>14</v>
       </c>
       <c r="B217" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C217" s="59" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D217" s="59" t="s">
         <v>1395</v>
-      </c>
-      <c r="D217" s="59" t="s">
-        <v>1396</v>
       </c>
       <c r="E217" s="119" t="n">
         <v>-1</v>
@@ -19211,13 +19205,13 @@
         <v>14</v>
       </c>
       <c r="B218" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C218" s="59" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D218" s="59" t="s">
         <v>1397</v>
-      </c>
-      <c r="D218" s="59" t="s">
-        <v>1398</v>
       </c>
       <c r="E218" s="119" t="n">
         <v>0</v>
@@ -19231,13 +19225,13 @@
         <v>14</v>
       </c>
       <c r="B219" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C219" s="59" t="s">
+        <v>1398</v>
+      </c>
+      <c r="D219" s="59" t="s">
         <v>1399</v>
-      </c>
-      <c r="D219" s="59" t="s">
-        <v>1400</v>
       </c>
       <c r="E219" s="119" t="n">
         <v>1</v>
@@ -19251,13 +19245,13 @@
         <v>14</v>
       </c>
       <c r="B220" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C220" s="59" t="s">
+        <v>1400</v>
+      </c>
+      <c r="D220" s="59" t="s">
         <v>1401</v>
-      </c>
-      <c r="D220" s="59" t="s">
-        <v>1402</v>
       </c>
       <c r="E220" s="119" t="n">
         <v>-1</v>
@@ -19271,13 +19265,13 @@
         <v>14</v>
       </c>
       <c r="B221" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C221" s="59" t="s">
+        <v>1402</v>
+      </c>
+      <c r="D221" s="59" t="s">
         <v>1403</v>
-      </c>
-      <c r="D221" s="59" t="s">
-        <v>1404</v>
       </c>
       <c r="E221" s="119" t="n">
         <v>1</v>
@@ -19291,13 +19285,13 @@
         <v>14</v>
       </c>
       <c r="B222" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C222" s="59" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D222" s="59" t="s">
         <v>1405</v>
-      </c>
-      <c r="D222" s="59" t="s">
-        <v>1406</v>
       </c>
       <c r="E222" s="119" t="n">
         <v>-1</v>
@@ -19311,13 +19305,13 @@
         <v>14</v>
       </c>
       <c r="B223" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C223" s="59" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D223" s="59" t="s">
         <v>1407</v>
-      </c>
-      <c r="D223" s="59" t="s">
-        <v>1408</v>
       </c>
       <c r="E223" s="119" t="n">
         <v>0</v>
@@ -19331,13 +19325,13 @@
         <v>14</v>
       </c>
       <c r="B224" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C224" s="59" t="s">
+        <v>1408</v>
+      </c>
+      <c r="D224" s="59" t="s">
         <v>1409</v>
-      </c>
-      <c r="D224" s="59" t="s">
-        <v>1410</v>
       </c>
       <c r="E224" s="119" t="n">
         <v>0</v>
@@ -19351,13 +19345,13 @@
         <v>14</v>
       </c>
       <c r="B225" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C225" s="59" t="s">
+        <v>1410</v>
+      </c>
+      <c r="D225" s="59" t="s">
         <v>1411</v>
-      </c>
-      <c r="D225" s="59" t="s">
-        <v>1412</v>
       </c>
       <c r="E225" s="119" t="n">
         <v>-1</v>
@@ -19371,13 +19365,13 @@
         <v>14</v>
       </c>
       <c r="B226" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C226" s="59" t="s">
+        <v>1412</v>
+      </c>
+      <c r="D226" s="59" t="s">
         <v>1413</v>
-      </c>
-      <c r="D226" s="59" t="s">
-        <v>1414</v>
       </c>
       <c r="E226" s="119" t="n">
         <v>0</v>
@@ -19391,13 +19385,13 @@
         <v>14</v>
       </c>
       <c r="B227" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C227" s="59" t="s">
+        <v>1414</v>
+      </c>
+      <c r="D227" s="59" t="s">
         <v>1415</v>
-      </c>
-      <c r="D227" s="59" t="s">
-        <v>1416</v>
       </c>
       <c r="E227" s="119" t="n">
         <v>1</v>
@@ -19411,13 +19405,13 @@
         <v>14</v>
       </c>
       <c r="B228" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C228" s="59" t="s">
+        <v>1416</v>
+      </c>
+      <c r="D228" s="59" t="s">
         <v>1417</v>
-      </c>
-      <c r="D228" s="59" t="s">
-        <v>1418</v>
       </c>
       <c r="E228" s="119" t="n">
         <v>-1</v>
@@ -19431,13 +19425,13 @@
         <v>14</v>
       </c>
       <c r="B229" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C229" s="59" t="s">
+        <v>1418</v>
+      </c>
+      <c r="D229" s="59" t="s">
         <v>1419</v>
-      </c>
-      <c r="D229" s="59" t="s">
-        <v>1420</v>
       </c>
       <c r="E229" s="119" t="n">
         <v>0</v>
@@ -19451,13 +19445,13 @@
         <v>14</v>
       </c>
       <c r="B230" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C230" s="59" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D230" s="59" t="s">
         <v>1421</v>
-      </c>
-      <c r="D230" s="59" t="s">
-        <v>1422</v>
       </c>
       <c r="E230" s="119" t="n">
         <v>-1</v>
@@ -19471,13 +19465,13 @@
         <v>14</v>
       </c>
       <c r="B231" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C231" s="59" t="s">
+        <v>1422</v>
+      </c>
+      <c r="D231" s="59" t="s">
         <v>1423</v>
-      </c>
-      <c r="D231" s="59" t="s">
-        <v>1424</v>
       </c>
       <c r="E231" s="119" t="n">
         <v>0</v>
@@ -19491,13 +19485,13 @@
         <v>14</v>
       </c>
       <c r="B232" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C232" s="59" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D232" s="59" t="s">
         <v>1425</v>
-      </c>
-      <c r="D232" s="59" t="s">
-        <v>1426</v>
       </c>
       <c r="E232" s="119" t="n">
         <v>0</v>
@@ -19511,13 +19505,13 @@
         <v>14</v>
       </c>
       <c r="B233" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C233" s="59" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D233" s="59" t="s">
         <v>1427</v>
-      </c>
-      <c r="D233" s="59" t="s">
-        <v>1428</v>
       </c>
       <c r="E233" s="119" t="n">
         <v>1</v>
@@ -19531,13 +19525,13 @@
         <v>14</v>
       </c>
       <c r="B234" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C234" s="59" t="s">
+        <v>1428</v>
+      </c>
+      <c r="D234" s="59" t="s">
         <v>1429</v>
-      </c>
-      <c r="D234" s="59" t="s">
-        <v>1430</v>
       </c>
       <c r="E234" s="119" t="n">
         <v>0</v>
@@ -19551,13 +19545,13 @@
         <v>14</v>
       </c>
       <c r="B235" s="139" t="s">
-        <v>1392</v>
+        <v>1391</v>
       </c>
       <c r="C235" s="59" t="s">
+        <v>1430</v>
+      </c>
+      <c r="D235" s="59" t="s">
         <v>1431</v>
-      </c>
-      <c r="D235" s="59" t="s">
-        <v>1432</v>
       </c>
       <c r="E235" s="119" t="n">
         <v>1</v>
@@ -19570,14 +19564,14 @@
       <c r="A236" s="87" t="n">
         <v>14</v>
       </c>
-      <c r="B236" s="150" t="s">
-        <v>1392</v>
+      <c r="B236" s="149" t="s">
+        <v>1391</v>
       </c>
       <c r="C236" s="103" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D236" s="103" t="s">
         <v>1433</v>
-      </c>
-      <c r="D236" s="103" t="s">
-        <v>1434</v>
       </c>
       <c r="E236" s="125" t="n">
         <v>0</v>
@@ -19591,13 +19585,13 @@
         <v>14</v>
       </c>
       <c r="B237" s="139" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C237" s="59" t="s">
         <v>1435</v>
       </c>
-      <c r="C237" s="59" t="s">
+      <c r="D237" s="59" t="s">
         <v>1436</v>
-      </c>
-      <c r="D237" s="59" t="s">
-        <v>1437</v>
       </c>
       <c r="E237" s="119" t="n">
         <v>-1</v>
@@ -19611,13 +19605,13 @@
         <v>14</v>
       </c>
       <c r="B238" s="139" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="C238" s="59" t="s">
+        <v>1437</v>
+      </c>
+      <c r="D238" s="59" t="s">
         <v>1438</v>
-      </c>
-      <c r="D238" s="59" t="s">
-        <v>1439</v>
       </c>
       <c r="E238" s="119" t="n">
         <v>-1</v>
@@ -19631,13 +19625,13 @@
         <v>14</v>
       </c>
       <c r="B239" s="139" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="C239" s="59" t="s">
+        <v>1439</v>
+      </c>
+      <c r="D239" s="59" t="s">
         <v>1440</v>
-      </c>
-      <c r="D239" s="59" t="s">
-        <v>1441</v>
       </c>
       <c r="E239" s="119" t="n">
         <v>1</v>
@@ -19651,13 +19645,13 @@
         <v>14</v>
       </c>
       <c r="B240" s="139" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="C240" s="59" t="s">
+        <v>1441</v>
+      </c>
+      <c r="D240" s="59" t="s">
         <v>1442</v>
-      </c>
-      <c r="D240" s="59" t="s">
-        <v>1443</v>
       </c>
       <c r="E240" s="119" t="n">
         <v>0</v>
@@ -19671,13 +19665,13 @@
         <v>14</v>
       </c>
       <c r="B241" s="139" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="C241" s="59" t="s">
+        <v>1443</v>
+      </c>
+      <c r="D241" s="59" t="s">
         <v>1444</v>
-      </c>
-      <c r="D241" s="59" t="s">
-        <v>1445</v>
       </c>
       <c r="E241" s="119" t="n">
         <v>0</v>
@@ -19691,13 +19685,13 @@
         <v>14</v>
       </c>
       <c r="B242" s="139" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="C242" s="59" t="s">
+        <v>1445</v>
+      </c>
+      <c r="D242" s="59" t="s">
         <v>1446</v>
-      </c>
-      <c r="D242" s="59" t="s">
-        <v>1447</v>
       </c>
       <c r="E242" s="119" t="n">
         <v>1</v>
@@ -19710,14 +19704,14 @@
       <c r="A243" s="87" t="n">
         <v>14</v>
       </c>
-      <c r="B243" s="150" t="s">
-        <v>1435</v>
+      <c r="B243" s="149" t="s">
+        <v>1434</v>
       </c>
       <c r="C243" s="103" t="s">
+        <v>1447</v>
+      </c>
+      <c r="D243" s="103" t="s">
         <v>1448</v>
-      </c>
-      <c r="D243" s="103" t="s">
-        <v>1449</v>
       </c>
       <c r="E243" s="125" t="n">
         <v>0</v>
@@ -19731,13 +19725,13 @@
         <v>14</v>
       </c>
       <c r="B244" s="139" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C244" s="59" t="s">
         <v>1450</v>
       </c>
-      <c r="C244" s="59" t="s">
+      <c r="D244" s="59" t="s">
         <v>1451</v>
-      </c>
-      <c r="D244" s="59" t="s">
-        <v>1452</v>
       </c>
       <c r="E244" s="119" t="n">
         <v>0</v>
@@ -19751,13 +19745,13 @@
         <v>14</v>
       </c>
       <c r="B245" s="139" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="C245" s="59" t="s">
+        <v>1452</v>
+      </c>
+      <c r="D245" s="59" t="s">
         <v>1453</v>
-      </c>
-      <c r="D245" s="59" t="s">
-        <v>1454</v>
       </c>
       <c r="E245" s="119" t="n">
         <v>0</v>
@@ -19771,13 +19765,13 @@
         <v>14</v>
       </c>
       <c r="B246" s="139" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="C246" s="59" t="s">
+        <v>1454</v>
+      </c>
+      <c r="D246" s="59" t="s">
         <v>1455</v>
-      </c>
-      <c r="D246" s="59" t="s">
-        <v>1456</v>
       </c>
       <c r="E246" s="119" t="n">
         <v>1</v>
@@ -19791,13 +19785,13 @@
         <v>14</v>
       </c>
       <c r="B247" s="139" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="C247" s="59" t="s">
+        <v>1456</v>
+      </c>
+      <c r="D247" s="59" t="s">
         <v>1457</v>
-      </c>
-      <c r="D247" s="59" t="s">
-        <v>1458</v>
       </c>
       <c r="E247" s="119" t="n">
         <v>-1</v>
@@ -19811,13 +19805,13 @@
         <v>14</v>
       </c>
       <c r="B248" s="139" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="C248" s="59" t="s">
+        <v>1458</v>
+      </c>
+      <c r="D248" s="59" t="s">
         <v>1459</v>
-      </c>
-      <c r="D248" s="59" t="s">
-        <v>1460</v>
       </c>
       <c r="E248" s="119" t="n">
         <v>1</v>
@@ -19831,13 +19825,13 @@
         <v>14</v>
       </c>
       <c r="B249" s="140" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="C249" s="67" t="s">
+        <v>1460</v>
+      </c>
+      <c r="D249" s="67" t="s">
         <v>1461</v>
-      </c>
-      <c r="D249" s="67" t="s">
-        <v>1462</v>
       </c>
       <c r="E249" s="126" t="n">
         <v>0</v>
@@ -19851,13 +19845,13 @@
         <v>15</v>
       </c>
       <c r="B250" s="139" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C250" s="59" t="s">
         <v>1463</v>
       </c>
-      <c r="C250" s="59" t="s">
+      <c r="D250" s="59" t="s">
         <v>1464</v>
-      </c>
-      <c r="D250" s="59" t="s">
-        <v>1465</v>
       </c>
       <c r="E250" s="119" t="n">
         <v>0</v>
@@ -19871,13 +19865,13 @@
         <v>15</v>
       </c>
       <c r="B251" s="139" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="C251" s="59" t="s">
+        <v>1465</v>
+      </c>
+      <c r="D251" s="59" t="s">
         <v>1466</v>
-      </c>
-      <c r="D251" s="59" t="s">
-        <v>1467</v>
       </c>
       <c r="E251" s="119" t="n">
         <v>1</v>
@@ -19891,13 +19885,13 @@
         <v>15</v>
       </c>
       <c r="B252" s="139" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="C252" s="59" t="s">
+        <v>1467</v>
+      </c>
+      <c r="D252" s="59" t="s">
         <v>1468</v>
-      </c>
-      <c r="D252" s="59" t="s">
-        <v>1469</v>
       </c>
       <c r="E252" s="119" t="n">
         <v>0</v>
@@ -19911,13 +19905,13 @@
         <v>15</v>
       </c>
       <c r="B253" s="139" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="C253" s="59" t="s">
+        <v>1469</v>
+      </c>
+      <c r="D253" s="59" t="s">
         <v>1470</v>
-      </c>
-      <c r="D253" s="59" t="s">
-        <v>1471</v>
       </c>
       <c r="E253" s="119" t="n">
         <v>0</v>
@@ -19931,13 +19925,13 @@
         <v>15</v>
       </c>
       <c r="B254" s="139" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="C254" s="59" t="s">
+        <v>1471</v>
+      </c>
+      <c r="D254" s="59" t="s">
         <v>1472</v>
-      </c>
-      <c r="D254" s="59" t="s">
-        <v>1473</v>
       </c>
       <c r="E254" s="119" t="n">
         <v>0</v>
@@ -19951,13 +19945,13 @@
         <v>15</v>
       </c>
       <c r="B255" s="139" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="C255" s="59" t="s">
+        <v>1473</v>
+      </c>
+      <c r="D255" s="59" t="s">
         <v>1474</v>
-      </c>
-      <c r="D255" s="59" t="s">
-        <v>1475</v>
       </c>
       <c r="E255" s="119" t="n">
         <v>1</v>
@@ -19971,13 +19965,13 @@
         <v>15</v>
       </c>
       <c r="B256" s="139" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="C256" s="59" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D256" s="59" t="s">
         <v>1476</v>
-      </c>
-      <c r="D256" s="59" t="s">
-        <v>1477</v>
       </c>
       <c r="E256" s="119" t="n">
         <v>-1</v>
@@ -19991,13 +19985,13 @@
         <v>15</v>
       </c>
       <c r="B257" s="139" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="C257" s="59" t="s">
+        <v>1477</v>
+      </c>
+      <c r="D257" s="59" t="s">
         <v>1478</v>
-      </c>
-      <c r="D257" s="59" t="s">
-        <v>1479</v>
       </c>
       <c r="E257" s="119" t="n">
         <v>0</v>
@@ -20011,13 +20005,13 @@
         <v>15</v>
       </c>
       <c r="B258" s="139" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="C258" s="59" t="s">
+        <v>1479</v>
+      </c>
+      <c r="D258" s="59" t="s">
         <v>1480</v>
-      </c>
-      <c r="D258" s="59" t="s">
-        <v>1481</v>
       </c>
       <c r="E258" s="119" t="n">
         <v>-1</v>
@@ -20031,13 +20025,13 @@
         <v>15</v>
       </c>
       <c r="B259" s="139" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="C259" s="59" t="s">
+        <v>1481</v>
+      </c>
+      <c r="D259" s="59" t="s">
         <v>1482</v>
-      </c>
-      <c r="D259" s="59" t="s">
-        <v>1483</v>
       </c>
       <c r="E259" s="119" t="n">
         <v>0</v>
@@ -20047,22 +20041,22 @@
       </c>
     </row>
     <row r="260" customFormat="false" ht="82.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="151" t="n">
+      <c r="A260" s="150" t="n">
         <v>15</v>
       </c>
-      <c r="B260" s="152" t="s">
-        <v>1463</v>
-      </c>
-      <c r="C260" s="153" t="s">
+      <c r="B260" s="151" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C260" s="145" t="s">
+        <v>1483</v>
+      </c>
+      <c r="D260" s="145" t="s">
         <v>1484</v>
       </c>
-      <c r="D260" s="153" t="s">
-        <v>1485</v>
-      </c>
-      <c r="E260" s="154" t="n">
-        <v>1</v>
-      </c>
-      <c r="F260" s="154" t="n">
+      <c r="E260" s="152" t="n">
+        <v>1</v>
+      </c>
+      <c r="F260" s="152" t="n">
         <v>1</v>
       </c>
     </row>
@@ -20070,14 +20064,14 @@
       <c r="A261" s="87" t="n">
         <v>15</v>
       </c>
-      <c r="B261" s="150" t="s">
-        <v>1463</v>
+      <c r="B261" s="149" t="s">
+        <v>1462</v>
       </c>
       <c r="C261" s="103" t="s">
+        <v>1485</v>
+      </c>
+      <c r="D261" s="103" t="s">
         <v>1486</v>
-      </c>
-      <c r="D261" s="103" t="s">
-        <v>1487</v>
       </c>
       <c r="E261" s="125" t="n">
         <v>0</v>
@@ -20091,13 +20085,13 @@
         <v>15</v>
       </c>
       <c r="B262" s="139" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C262" s="59" t="s">
         <v>1488</v>
       </c>
-      <c r="C262" s="59" t="s">
+      <c r="D262" s="59" t="s">
         <v>1489</v>
-      </c>
-      <c r="D262" s="59" t="s">
-        <v>1490</v>
       </c>
       <c r="E262" s="119" t="n">
         <v>-1</v>
@@ -20111,13 +20105,13 @@
         <v>15</v>
       </c>
       <c r="B263" s="139" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C263" s="59" t="s">
+        <v>1490</v>
+      </c>
+      <c r="D263" s="59" t="s">
         <v>1491</v>
-      </c>
-      <c r="D263" s="59" t="s">
-        <v>1492</v>
       </c>
       <c r="E263" s="119" t="n">
         <v>-1</v>
@@ -20131,13 +20125,13 @@
         <v>15</v>
       </c>
       <c r="B264" s="139" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C264" s="59" t="s">
+        <v>1492</v>
+      </c>
+      <c r="D264" s="59" t="s">
         <v>1493</v>
-      </c>
-      <c r="D264" s="59" t="s">
-        <v>1494</v>
       </c>
       <c r="E264" s="119" t="n">
         <v>-1</v>
@@ -20151,13 +20145,13 @@
         <v>15</v>
       </c>
       <c r="B265" s="139" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C265" s="59" t="s">
+        <v>1494</v>
+      </c>
+      <c r="D265" s="59" t="s">
         <v>1495</v>
-      </c>
-      <c r="D265" s="59" t="s">
-        <v>1496</v>
       </c>
       <c r="E265" s="119" t="n">
         <v>0</v>
@@ -20171,13 +20165,13 @@
         <v>15</v>
       </c>
       <c r="B266" s="139" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C266" s="59" t="s">
+        <v>1496</v>
+      </c>
+      <c r="D266" s="59" t="s">
         <v>1497</v>
-      </c>
-      <c r="D266" s="59" t="s">
-        <v>1498</v>
       </c>
       <c r="E266" s="119" t="n">
         <v>0</v>
@@ -20191,13 +20185,13 @@
         <v>15</v>
       </c>
       <c r="B267" s="139" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C267" s="59" t="s">
+        <v>1498</v>
+      </c>
+      <c r="D267" s="59" t="s">
         <v>1499</v>
-      </c>
-      <c r="D267" s="59" t="s">
-        <v>1500</v>
       </c>
       <c r="E267" s="119" t="n">
         <v>-1</v>
@@ -20211,13 +20205,13 @@
         <v>15</v>
       </c>
       <c r="B268" s="139" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C268" s="59" t="s">
+        <v>1500</v>
+      </c>
+      <c r="D268" s="59" t="s">
         <v>1501</v>
-      </c>
-      <c r="D268" s="59" t="s">
-        <v>1502</v>
       </c>
       <c r="E268" s="119" t="n">
         <v>-1</v>
@@ -20231,13 +20225,13 @@
         <v>15</v>
       </c>
       <c r="B269" s="139" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C269" s="59" t="s">
+        <v>1502</v>
+      </c>
+      <c r="D269" s="59" t="s">
         <v>1503</v>
-      </c>
-      <c r="D269" s="59" t="s">
-        <v>1504</v>
       </c>
       <c r="E269" s="119" t="n">
         <v>-1</v>
@@ -20251,13 +20245,13 @@
         <v>15</v>
       </c>
       <c r="B270" s="139" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C270" s="59" t="s">
+        <v>1504</v>
+      </c>
+      <c r="D270" s="59" t="s">
         <v>1505</v>
-      </c>
-      <c r="D270" s="59" t="s">
-        <v>1506</v>
       </c>
       <c r="E270" s="119" t="n">
         <v>0</v>
@@ -20271,13 +20265,13 @@
         <v>15</v>
       </c>
       <c r="B271" s="139" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C271" s="59" t="s">
+        <v>1506</v>
+      </c>
+      <c r="D271" s="59" t="s">
         <v>1507</v>
-      </c>
-      <c r="D271" s="59" t="s">
-        <v>1508</v>
       </c>
       <c r="E271" s="119" t="n">
         <v>0</v>
@@ -20290,14 +20284,14 @@
       <c r="A272" s="87" t="n">
         <v>15</v>
       </c>
-      <c r="B272" s="150" t="s">
-        <v>1488</v>
+      <c r="B272" s="149" t="s">
+        <v>1487</v>
       </c>
       <c r="C272" s="103" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D272" s="103" t="s">
         <v>1509</v>
-      </c>
-      <c r="D272" s="103" t="s">
-        <v>1510</v>
       </c>
       <c r="E272" s="125" t="n">
         <v>-1</v>
@@ -20311,13 +20305,13 @@
         <v>15</v>
       </c>
       <c r="B273" s="139" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C273" s="59" t="s">
         <v>1511</v>
       </c>
-      <c r="C273" s="59" t="s">
+      <c r="D273" s="59" t="s">
         <v>1512</v>
-      </c>
-      <c r="D273" s="59" t="s">
-        <v>1513</v>
       </c>
       <c r="E273" s="119" t="n">
         <v>0</v>
@@ -20327,57 +20321,57 @@
       </c>
     </row>
     <row r="274" customFormat="false" ht="96.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="151" t="n">
+      <c r="A274" s="150" t="n">
         <v>15</v>
       </c>
       <c r="B274" s="139" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="C274" s="59" t="s">
+        <v>1513</v>
+      </c>
+      <c r="D274" s="59" t="s">
         <v>1514</v>
       </c>
-      <c r="D274" s="59" t="s">
+      <c r="E274" s="119" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F274" s="119" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="96.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A275" s="150" t="n">
+        <v>15</v>
+      </c>
+      <c r="B275" s="139" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C275" s="59" t="s">
         <v>1515</v>
       </c>
-      <c r="E274" s="119" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F274" s="119" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="275" customFormat="false" ht="96.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="151" t="n">
+      <c r="D275" s="59" t="s">
+        <v>1516</v>
+      </c>
+      <c r="E275" s="119" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F275" s="119" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="276" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A276" s="150" t="n">
         <v>15</v>
       </c>
-      <c r="B275" s="139" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C275" s="59" t="s">
-        <v>1516</v>
-      </c>
-      <c r="D275" s="59" t="s">
+      <c r="B276" s="139" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C276" s="59" t="s">
         <v>1517</v>
       </c>
-      <c r="E275" s="119" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F275" s="119" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="276" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="151" t="n">
-        <v>15</v>
-      </c>
-      <c r="B276" s="139" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C276" s="59" t="s">
+      <c r="D276" s="59" t="s">
         <v>1518</v>
-      </c>
-      <c r="D276" s="59" t="s">
-        <v>1519</v>
       </c>
       <c r="E276" s="119" t="n">
         <v>0</v>
@@ -20387,117 +20381,117 @@
       </c>
     </row>
     <row r="277" customFormat="false" ht="82.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="151" t="n">
+      <c r="A277" s="150" t="n">
         <v>15</v>
       </c>
       <c r="B277" s="139" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="C277" s="59" t="s">
+        <v>1519</v>
+      </c>
+      <c r="D277" s="59" t="s">
         <v>1520</v>
       </c>
-      <c r="D277" s="59" t="s">
+      <c r="E277" s="119" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F277" s="119" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="278" customFormat="false" ht="82.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A278" s="150" t="n">
+        <v>15</v>
+      </c>
+      <c r="B278" s="139" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C278" s="59" t="s">
         <v>1521</v>
       </c>
-      <c r="E277" s="119" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F277" s="119" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="278" customFormat="false" ht="82.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="151" t="n">
+      <c r="D278" s="59" t="s">
+        <v>1522</v>
+      </c>
+      <c r="E278" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="F278" s="119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" customFormat="false" ht="96.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A279" s="150" t="n">
         <v>15</v>
       </c>
-      <c r="B278" s="139" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C278" s="59" t="s">
-        <v>1522</v>
-      </c>
-      <c r="D278" s="59" t="s">
+      <c r="B279" s="139" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C279" s="59" t="s">
         <v>1523</v>
       </c>
-      <c r="E278" s="119" t="n">
-        <v>1</v>
-      </c>
-      <c r="F278" s="119" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="279" customFormat="false" ht="96.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="151" t="n">
+      <c r="D279" s="59" t="s">
+        <v>1524</v>
+      </c>
+      <c r="E279" s="119" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F279" s="119" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="280" customFormat="false" ht="96.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A280" s="150" t="n">
         <v>15</v>
       </c>
-      <c r="B279" s="139" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C279" s="59" t="s">
-        <v>1524</v>
-      </c>
-      <c r="D279" s="59" t="s">
+      <c r="B280" s="139" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C280" s="59" t="s">
         <v>1525</v>
       </c>
-      <c r="E279" s="119" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F279" s="119" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="280" customFormat="false" ht="96.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="151" t="n">
+      <c r="D280" s="59" t="s">
+        <v>1526</v>
+      </c>
+      <c r="E280" s="119" t="n">
+        <v>-1</v>
+      </c>
+      <c r="F280" s="119" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="281" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A281" s="150" t="n">
         <v>15</v>
       </c>
-      <c r="B280" s="139" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C280" s="59" t="s">
-        <v>1526</v>
-      </c>
-      <c r="D280" s="59" t="s">
+      <c r="B281" s="139" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C281" s="59" t="s">
         <v>1527</v>
       </c>
-      <c r="E280" s="119" t="n">
-        <v>-1</v>
-      </c>
-      <c r="F280" s="119" t="n">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="281" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="151" t="n">
+      <c r="D281" s="59" t="s">
+        <v>1528</v>
+      </c>
+      <c r="E281" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="F281" s="119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" customFormat="false" ht="96.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A282" s="150" t="n">
         <v>15</v>
       </c>
-      <c r="B281" s="139" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C281" s="59" t="s">
-        <v>1528</v>
-      </c>
-      <c r="D281" s="59" t="s">
+      <c r="B282" s="139" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C282" s="59" t="s">
         <v>1529</v>
       </c>
-      <c r="E281" s="119" t="n">
-        <v>1</v>
-      </c>
-      <c r="F281" s="119" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="282" customFormat="false" ht="96.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="151" t="n">
-        <v>15</v>
-      </c>
-      <c r="B282" s="139" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C282" s="59" t="s">
+      <c r="D282" s="59" t="s">
         <v>1530</v>
-      </c>
-      <c r="D282" s="59" t="s">
-        <v>1531</v>
       </c>
       <c r="E282" s="119" t="n">
         <v>0</v>
@@ -20507,37 +20501,37 @@
       </c>
     </row>
     <row r="283" customFormat="false" ht="122.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="151" t="n">
+      <c r="A283" s="150" t="n">
         <v>15</v>
       </c>
       <c r="B283" s="139" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="C283" s="59" t="s">
+        <v>1531</v>
+      </c>
+      <c r="D283" s="59" t="s">
         <v>1532</v>
       </c>
-      <c r="D283" s="59" t="s">
+      <c r="E283" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="F283" s="119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A284" s="150" t="n">
+        <v>15</v>
+      </c>
+      <c r="B284" s="139" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C284" s="59" t="s">
         <v>1533</v>
       </c>
-      <c r="E283" s="119" t="n">
-        <v>1</v>
-      </c>
-      <c r="F283" s="119" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="284" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="151" t="n">
-        <v>15</v>
-      </c>
-      <c r="B284" s="139" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C284" s="59" t="s">
+      <c r="D284" s="59" t="s">
         <v>1534</v>
-      </c>
-      <c r="D284" s="59" t="s">
-        <v>1535</v>
       </c>
       <c r="E284" s="119" t="n">
         <v>0</v>
@@ -20547,57 +20541,57 @@
       </c>
     </row>
     <row r="285" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="151" t="n">
+      <c r="A285" s="150" t="n">
         <v>15</v>
       </c>
       <c r="B285" s="139" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="C285" s="59" t="s">
+        <v>1535</v>
+      </c>
+      <c r="D285" s="59" t="s">
         <v>1536</v>
       </c>
-      <c r="D285" s="59" t="s">
+      <c r="E285" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="F285" s="119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="150" t="n">
+        <v>15</v>
+      </c>
+      <c r="B286" s="139" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C286" s="59" t="s">
         <v>1537</v>
       </c>
-      <c r="E285" s="119" t="n">
-        <v>1</v>
-      </c>
-      <c r="F285" s="119" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="286" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="151" t="n">
+      <c r="D286" s="59" t="s">
+        <v>1538</v>
+      </c>
+      <c r="E286" s="119" t="n">
+        <v>1</v>
+      </c>
+      <c r="F286" s="119" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" customFormat="false" ht="82.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A287" s="150" t="n">
         <v>15</v>
       </c>
-      <c r="B286" s="139" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C286" s="59" t="s">
-        <v>1538</v>
-      </c>
-      <c r="D286" s="59" t="s">
+      <c r="B287" s="139" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C287" s="59" t="s">
         <v>1539</v>
       </c>
-      <c r="E286" s="119" t="n">
-        <v>1</v>
-      </c>
-      <c r="F286" s="119" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="287" customFormat="false" ht="82.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="151" t="n">
-        <v>15</v>
-      </c>
-      <c r="B287" s="139" t="s">
-        <v>1511</v>
-      </c>
-      <c r="C287" s="59" t="s">
+      <c r="D287" s="59" t="s">
         <v>1540</v>
-      </c>
-      <c r="D287" s="59" t="s">
-        <v>1541</v>
       </c>
       <c r="E287" s="119" t="n">
         <v>0</v>
@@ -20607,17 +20601,17 @@
       </c>
     </row>
     <row r="288" customFormat="false" ht="96.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="151" t="n">
+      <c r="A288" s="150" t="n">
         <v>15</v>
       </c>
       <c r="B288" s="139" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="C288" s="59" t="s">
+        <v>1541</v>
+      </c>
+      <c r="D288" s="59" t="s">
         <v>1542</v>
-      </c>
-      <c r="D288" s="59" t="s">
-        <v>1543</v>
       </c>
       <c r="E288" s="119" t="n">
         <v>0</v>
@@ -20627,17 +20621,17 @@
       </c>
     </row>
     <row r="289" customFormat="false" ht="69.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="151" t="n">
+      <c r="A289" s="150" t="n">
         <v>15</v>
       </c>
       <c r="B289" s="139" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="C289" s="59" t="s">
+        <v>1543</v>
+      </c>
+      <c r="D289" s="59" t="s">
         <v>1544</v>
-      </c>
-      <c r="D289" s="59" t="s">
-        <v>1545</v>
       </c>
       <c r="E289" s="119" t="n">
         <v>1</v>
@@ -20650,14 +20644,14 @@
       <c r="A290" s="87" t="n">
         <v>15</v>
       </c>
-      <c r="B290" s="150" t="s">
-        <v>1511</v>
+      <c r="B290" s="149" t="s">
+        <v>1510</v>
       </c>
       <c r="C290" s="103" t="s">
+        <v>1545</v>
+      </c>
+      <c r="D290" s="103" t="s">
         <v>1546</v>
-      </c>
-      <c r="D290" s="103" t="s">
-        <v>1547</v>
       </c>
       <c r="E290" s="125" t="n">
         <v>0</v>
@@ -20671,13 +20665,13 @@
         <v>15</v>
       </c>
       <c r="B291" s="139" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C291" s="59" t="s">
         <v>1548</v>
       </c>
-      <c r="C291" s="59" t="s">
+      <c r="D291" s="59" t="s">
         <v>1549</v>
-      </c>
-      <c r="D291" s="59" t="s">
-        <v>1550</v>
       </c>
       <c r="E291" s="119" t="n">
         <v>0</v>
@@ -20691,13 +20685,13 @@
         <v>15</v>
       </c>
       <c r="B292" s="139" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C292" s="59" t="s">
+        <v>1550</v>
+      </c>
+      <c r="D292" s="59" t="s">
         <v>1551</v>
-      </c>
-      <c r="D292" s="59" t="s">
-        <v>1552</v>
       </c>
       <c r="E292" s="119" t="n">
         <v>1</v>
@@ -20711,13 +20705,13 @@
         <v>15</v>
       </c>
       <c r="B293" s="139" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C293" s="59" t="s">
+        <v>1552</v>
+      </c>
+      <c r="D293" s="59" t="s">
         <v>1553</v>
-      </c>
-      <c r="D293" s="59" t="s">
-        <v>1554</v>
       </c>
       <c r="E293" s="119" t="n">
         <v>0</v>
@@ -20731,13 +20725,13 @@
         <v>15</v>
       </c>
       <c r="B294" s="139" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C294" s="59" t="s">
+        <v>1554</v>
+      </c>
+      <c r="D294" s="59" t="s">
         <v>1555</v>
-      </c>
-      <c r="D294" s="59" t="s">
-        <v>1556</v>
       </c>
       <c r="E294" s="119" t="n">
         <v>1</v>
@@ -20751,13 +20745,13 @@
         <v>15</v>
       </c>
       <c r="B295" s="139" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C295" s="59" t="s">
+        <v>1556</v>
+      </c>
+      <c r="D295" s="59" t="s">
         <v>1557</v>
-      </c>
-      <c r="D295" s="59" t="s">
-        <v>1558</v>
       </c>
       <c r="E295" s="119" t="n">
         <v>-1</v>
@@ -20771,13 +20765,13 @@
         <v>15</v>
       </c>
       <c r="B296" s="139" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C296" s="59" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="D296" s="59" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="E296" s="119" t="n">
         <v>1</v>
@@ -20791,13 +20785,13 @@
         <v>15</v>
       </c>
       <c r="B297" s="139" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C297" s="59" t="s">
+        <v>1559</v>
+      </c>
+      <c r="D297" s="59" t="s">
         <v>1560</v>
-      </c>
-      <c r="D297" s="59" t="s">
-        <v>1561</v>
       </c>
       <c r="E297" s="119" t="n">
         <v>0</v>
@@ -20811,13 +20805,13 @@
         <v>15</v>
       </c>
       <c r="B298" s="139" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C298" s="59" t="s">
+        <v>1561</v>
+      </c>
+      <c r="D298" s="59" t="s">
         <v>1562</v>
-      </c>
-      <c r="D298" s="59" t="s">
-        <v>1563</v>
       </c>
       <c r="E298" s="119" t="n">
         <v>0</v>
@@ -20831,13 +20825,13 @@
         <v>15</v>
       </c>
       <c r="B299" s="139" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C299" s="59" t="s">
+        <v>1563</v>
+      </c>
+      <c r="D299" s="59" t="s">
         <v>1564</v>
-      </c>
-      <c r="D299" s="59" t="s">
-        <v>1565</v>
       </c>
       <c r="E299" s="119" t="n">
         <v>0</v>
@@ -20851,13 +20845,13 @@
         <v>15</v>
       </c>
       <c r="B300" s="140" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="C300" s="67" t="s">
+        <v>1565</v>
+      </c>
+      <c r="D300" s="67" t="s">
         <v>1566</v>
-      </c>
-      <c r="D300" s="67" t="s">
-        <v>1567</v>
       </c>
       <c r="E300" s="126" t="n">
         <v>-1</v>
@@ -20894,8 +20888,8 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B72" activeCellId="0" sqref="B72"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A63" colorId="64" zoomScale="92" zoomScaleNormal="92" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A80" activeCellId="0" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -20907,28 +20901,28 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="153" t="s">
+        <v>1567</v>
+      </c>
+      <c r="B1" s="154" t="s">
         <v>1568</v>
       </c>
-      <c r="B1" s="156" t="s">
+      <c r="C1" s="154" t="s">
         <v>1569</v>
       </c>
-      <c r="C1" s="156" t="s">
-        <v>1570</v>
-      </c>
-      <c r="D1" s="157" t="s">
+      <c r="D1" s="155" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="59" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>433</v>
       </c>
       <c r="C2" s="58" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>1</v>
@@ -20936,13 +20930,13 @@
     </row>
     <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="59" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>443</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>1</v>
@@ -20950,13 +20944,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="59" t="s">
+        <v>1574</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>1575</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="58" t="s">
         <v>1576</v>
-      </c>
-      <c r="C4" s="58" t="s">
-        <v>1577</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>1</v>
@@ -20964,13 +20958,13 @@
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="59" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>477</v>
       </c>
       <c r="C5" s="58" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>1</v>
@@ -20978,13 +20972,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="B6" s="59" t="s">
         <v>480</v>
       </c>
       <c r="C6" s="58" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="D6" s="0" t="n">
         <v>1</v>
@@ -20992,13 +20986,13 @@
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>483</v>
       </c>
       <c r="C7" s="58" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>1</v>
@@ -21006,13 +21000,13 @@
     </row>
     <row r="8" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>1581</v>
-      </c>
-      <c r="B8" s="153" t="s">
+        <v>1580</v>
+      </c>
+      <c r="B8" s="145" t="s">
         <v>494</v>
       </c>
       <c r="C8" s="58" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>1</v>
@@ -21020,13 +21014,13 @@
     </row>
     <row r="9" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B9" s="95" t="s">
         <v>920</v>
       </c>
       <c r="C9" s="58" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>1</v>
@@ -21034,13 +21028,13 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>1583</v>
+      </c>
+      <c r="B10" s="156" t="s">
         <v>1584</v>
       </c>
-      <c r="B10" s="158" t="s">
+      <c r="C10" s="58" t="s">
         <v>1585</v>
-      </c>
-      <c r="C10" s="58" t="s">
-        <v>1586</v>
       </c>
       <c r="D10" s="0" t="n">
         <v>1</v>
@@ -21048,13 +21042,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>1587</v>
-      </c>
-      <c r="B11" s="158" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B11" s="156" t="s">
         <v>927</v>
       </c>
       <c r="C11" s="58" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>1</v>
@@ -21062,13 +21056,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="69" t="s">
-        <v>1588</v>
+        <v>1587</v>
       </c>
       <c r="B12" s="67" t="s">
         <v>934</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="D12" s="69" t="n">
         <v>1</v>
@@ -21076,27 +21070,27 @@
     </row>
     <row r="13" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="146" t="s">
-        <v>1590</v>
-      </c>
-      <c r="B13" s="153" t="s">
+        <v>1589</v>
+      </c>
+      <c r="B13" s="145" t="s">
         <v>508</v>
       </c>
-      <c r="C13" s="159" t="s">
-        <v>1574</v>
-      </c>
-      <c r="D13" s="160" t="n">
+      <c r="C13" s="157" t="s">
+        <v>1573</v>
+      </c>
+      <c r="D13" s="158" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="55.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="59" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="B14" s="59" t="s">
         <v>527</v>
       </c>
-      <c r="C14" s="161" t="s">
-        <v>1574</v>
+      <c r="C14" s="159" t="s">
+        <v>1573</v>
       </c>
       <c r="D14" s="146" t="n">
         <v>2</v>
@@ -21104,13 +21098,13 @@
     </row>
     <row r="15" customFormat="false" ht="162.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="59" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="B15" s="146" t="s">
         <v>534</v>
       </c>
-      <c r="C15" s="161" t="s">
-        <v>1574</v>
+      <c r="C15" s="159" t="s">
+        <v>1573</v>
       </c>
       <c r="D15" s="146" t="n">
         <v>2</v>
@@ -21118,13 +21112,13 @@
     </row>
     <row r="16" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="59" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B16" s="146" t="s">
         <v>1593</v>
       </c>
-      <c r="B16" s="146" t="s">
+      <c r="C16" s="159" t="s">
         <v>1594</v>
-      </c>
-      <c r="C16" s="161" t="s">
-        <v>1595</v>
       </c>
       <c r="D16" s="146" t="n">
         <v>2</v>
@@ -21132,13 +21126,13 @@
     </row>
     <row r="17" s="146" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="59" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
       <c r="B17" s="146" t="s">
         <v>939</v>
       </c>
-      <c r="C17" s="161" t="s">
-        <v>1589</v>
+      <c r="C17" s="159" t="s">
+        <v>1588</v>
       </c>
       <c r="D17" s="146" t="n">
         <v>2</v>
@@ -21146,13 +21140,13 @@
     </row>
     <row r="18" s="146" customFormat="true" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="146" t="s">
+        <v>1596</v>
+      </c>
+      <c r="B18" s="146" t="s">
         <v>1597</v>
       </c>
-      <c r="B18" s="146" t="s">
-        <v>1598</v>
-      </c>
-      <c r="C18" s="161" t="s">
-        <v>1589</v>
+      <c r="C18" s="159" t="s">
+        <v>1588</v>
       </c>
       <c r="D18" s="146" t="n">
         <v>2</v>
@@ -21160,13 +21154,13 @@
     </row>
     <row r="19" s="146" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="59" t="s">
+        <v>1598</v>
+      </c>
+      <c r="B19" s="146" t="s">
         <v>1599</v>
       </c>
-      <c r="B19" s="146" t="s">
+      <c r="C19" s="159" t="s">
         <v>1600</v>
-      </c>
-      <c r="C19" s="161" t="s">
-        <v>1601</v>
       </c>
       <c r="D19" s="146" t="n">
         <v>2</v>
@@ -21174,13 +21168,13 @@
     </row>
     <row r="20" s="146" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="99" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B20" s="148" t="s">
         <v>1602</v>
       </c>
-      <c r="B20" s="148" t="s">
-        <v>1603</v>
-      </c>
-      <c r="C20" s="162" t="s">
-        <v>1601</v>
+      <c r="C20" s="160" t="s">
+        <v>1600</v>
       </c>
       <c r="D20" s="148" t="n">
         <v>2</v>
@@ -21188,13 +21182,13 @@
     </row>
     <row r="21" s="146" customFormat="true" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>1604</v>
-      </c>
-      <c r="B21" s="163" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B21" s="161" t="s">
         <v>546</v>
       </c>
       <c r="C21" s="58" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>3</v>
@@ -21202,13 +21196,13 @@
     </row>
     <row r="22" s="146" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>1605</v>
-      </c>
-      <c r="B22" s="163" t="s">
+        <v>1604</v>
+      </c>
+      <c r="B22" s="161" t="s">
         <v>558</v>
       </c>
       <c r="C22" s="58" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>3</v>
@@ -21216,13 +21210,13 @@
     </row>
     <row r="23" s="146" customFormat="true" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>1606</v>
-      </c>
-      <c r="B23" s="163" t="s">
+        <v>1605</v>
+      </c>
+      <c r="B23" s="161" t="s">
         <v>561</v>
       </c>
       <c r="C23" s="58" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="D23" s="0" t="n">
         <v>3</v>
@@ -21230,13 +21224,13 @@
     </row>
     <row r="24" s="146" customFormat="true" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B24" s="161" t="s">
+        <v>582</v>
+      </c>
+      <c r="C24" s="58" t="s">
         <v>1607</v>
-      </c>
-      <c r="B24" s="163" t="s">
-        <v>582</v>
-      </c>
-      <c r="C24" s="58" t="s">
-        <v>1608</v>
       </c>
       <c r="D24" s="0" t="n">
         <v>3</v>
@@ -21244,13 +21238,13 @@
     </row>
     <row r="25" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>1608</v>
+      </c>
+      <c r="B25" s="161" t="s">
+        <v>589</v>
+      </c>
+      <c r="C25" s="58" t="s">
         <v>1609</v>
-      </c>
-      <c r="B25" s="163" t="s">
-        <v>589</v>
-      </c>
-      <c r="C25" s="58" t="s">
-        <v>1610</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>3</v>
@@ -21258,13 +21252,13 @@
     </row>
     <row r="26" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>1611</v>
-      </c>
-      <c r="B26" s="163" t="s">
+        <v>1610</v>
+      </c>
+      <c r="B26" s="161" t="s">
         <v>604</v>
       </c>
       <c r="C26" s="58" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="D26" s="0" t="n">
         <v>3</v>
@@ -21272,13 +21266,13 @@
     </row>
     <row r="27" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="59" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="B27" s="95" t="s">
         <v>977</v>
       </c>
       <c r="C27" s="58" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="D27" s="0" t="n">
         <v>3</v>
@@ -21286,13 +21280,13 @@
     </row>
     <row r="28" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="59" t="s">
-        <v>1614</v>
-      </c>
-      <c r="B28" s="158" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B28" s="156" t="s">
         <v>984</v>
       </c>
       <c r="C28" s="58" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="D28" s="0" t="n">
         <v>3</v>
@@ -21300,13 +21294,13 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="59" t="s">
-        <v>1615</v>
-      </c>
-      <c r="B29" s="158" t="s">
+        <v>1614</v>
+      </c>
+      <c r="B29" s="156" t="s">
         <v>989</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="D29" s="0" t="n">
         <v>3</v>
@@ -21314,13 +21308,13 @@
     </row>
     <row r="30" customFormat="false" ht="109.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="59" t="s">
+        <v>1615</v>
+      </c>
+      <c r="B30" s="156" t="s">
+        <v>994</v>
+      </c>
+      <c r="C30" s="58" t="s">
         <v>1616</v>
-      </c>
-      <c r="B30" s="158" t="s">
-        <v>994</v>
-      </c>
-      <c r="C30" s="58" t="s">
-        <v>1617</v>
       </c>
       <c r="D30" s="0" t="n">
         <v>3</v>
@@ -21328,13 +21322,13 @@
     </row>
     <row r="31" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="67" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B31" s="99" t="s">
         <v>1001</v>
       </c>
       <c r="C31" s="66" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="D31" s="69" t="n">
         <v>3</v>
@@ -21342,13 +21336,13 @@
     </row>
     <row r="32" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>1618</v>
+      </c>
+      <c r="B32" s="93" t="s">
         <v>1619</v>
       </c>
-      <c r="B32" s="93" t="s">
-        <v>1620</v>
-      </c>
-      <c r="C32" s="164" t="s">
-        <v>1595</v>
+      <c r="C32" s="162" t="s">
+        <v>1594</v>
       </c>
       <c r="D32" s="0" t="n">
         <v>4</v>
@@ -21356,13 +21350,13 @@
     </row>
     <row r="33" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="59" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="B33" s="95" t="s">
         <v>621</v>
       </c>
-      <c r="C33" s="164" t="s">
-        <v>1574</v>
+      <c r="C33" s="162" t="s">
+        <v>1573</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>4</v>
@@ -21370,13 +21364,13 @@
     </row>
     <row r="34" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="B34" s="59" t="s">
         <v>628</v>
       </c>
       <c r="C34" s="58" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="D34" s="0" t="n">
         <v>4</v>
@@ -21384,13 +21378,13 @@
     </row>
     <row r="35" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="B35" s="105" t="s">
         <v>639</v>
       </c>
       <c r="C35" s="58" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="D35" s="0" t="n">
         <v>4</v>
@@ -21398,13 +21392,13 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="B36" s="95" t="s">
         <v>1006</v>
       </c>
       <c r="C36" s="58" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="D36" s="0" t="n">
         <v>4</v>
@@ -21412,13 +21406,13 @@
     </row>
     <row r="37" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>1011</v>
       </c>
       <c r="C37" s="58" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="D37" s="0" t="n">
         <v>4</v>
@@ -21426,13 +21420,13 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="69" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="B38" s="69" t="s">
         <v>1018</v>
       </c>
       <c r="C38" s="66" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="D38" s="69" t="n">
         <v>4</v>
@@ -21440,13 +21434,13 @@
     </row>
     <row r="39" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="B39" s="93" t="s">
         <v>661</v>
       </c>
-      <c r="C39" s="164" t="s">
-        <v>1572</v>
+      <c r="C39" s="162" t="s">
+        <v>1571</v>
       </c>
       <c r="D39" s="0" t="n">
         <v>5</v>
@@ -21454,13 +21448,13 @@
     </row>
     <row r="40" customFormat="false" ht="69.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="59" t="s">
-        <v>1629</v>
-      </c>
-      <c r="B40" s="163" t="s">
+        <v>1628</v>
+      </c>
+      <c r="B40" s="161" t="s">
         <v>664</v>
       </c>
-      <c r="C40" s="164" t="s">
-        <v>1572</v>
+      <c r="C40" s="162" t="s">
+        <v>1571</v>
       </c>
       <c r="D40" s="0" t="n">
         <v>5</v>
@@ -21468,13 +21462,13 @@
     </row>
     <row r="41" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="B41" s="93" t="s">
         <v>667</v>
       </c>
-      <c r="C41" s="164" t="s">
-        <v>1595</v>
+      <c r="C41" s="162" t="s">
+        <v>1594</v>
       </c>
       <c r="D41" s="0" t="n">
         <v>5</v>
@@ -21482,13 +21476,13 @@
     </row>
     <row r="42" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
       <c r="B42" s="93" t="s">
         <v>676</v>
       </c>
-      <c r="C42" s="164" t="s">
-        <v>1574</v>
+      <c r="C42" s="162" t="s">
+        <v>1573</v>
       </c>
       <c r="D42" s="0" t="n">
         <v>5</v>
@@ -21496,13 +21490,13 @@
     </row>
     <row r="43" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
       <c r="B43" s="93" t="s">
         <v>687</v>
       </c>
-      <c r="C43" s="164" t="s">
-        <v>1577</v>
+      <c r="C43" s="162" t="s">
+        <v>1576</v>
       </c>
       <c r="D43" s="0" t="n">
         <v>5</v>
@@ -21510,13 +21504,13 @@
     </row>
     <row r="44" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="59" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
       <c r="B44" s="139" t="s">
         <v>1023</v>
       </c>
-      <c r="C44" s="164" t="s">
-        <v>1583</v>
+      <c r="C44" s="162" t="s">
+        <v>1582</v>
       </c>
       <c r="D44" s="0" t="n">
         <v>5</v>
@@ -21524,13 +21518,13 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>1634</v>
-      </c>
-      <c r="B45" s="163" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B45" s="161" t="s">
         <v>1032</v>
       </c>
-      <c r="C45" s="164" t="s">
-        <v>1601</v>
+      <c r="C45" s="162" t="s">
+        <v>1600</v>
       </c>
       <c r="D45" s="0" t="n">
         <v>5</v>
@@ -21538,13 +21532,13 @@
     </row>
     <row r="46" customFormat="false" ht="310.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="148" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
       <c r="B46" s="97" t="s">
         <v>1035</v>
       </c>
       <c r="C46" s="66" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="D46" s="69" t="n">
         <v>5</v>
@@ -21552,13 +21546,13 @@
     </row>
     <row r="47" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
       <c r="B47" s="59" t="s">
         <v>708</v>
       </c>
       <c r="C47" s="58" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="D47" s="0" t="n">
         <v>6</v>
@@ -21566,13 +21560,13 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="146" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
       <c r="B48" s="59" t="s">
         <v>753</v>
       </c>
       <c r="C48" s="58" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="D48" s="0" t="n">
         <v>6</v>
@@ -21580,13 +21574,13 @@
     </row>
     <row r="49" customFormat="false" ht="310.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="146" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
       <c r="B49" s="59" t="s">
         <v>782</v>
       </c>
       <c r="C49" s="58" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="D49" s="0" t="n">
         <v>6</v>
@@ -21594,13 +21588,13 @@
     </row>
     <row r="50" customFormat="false" ht="82.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="146" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="B50" s="95" t="s">
         <v>1048</v>
       </c>
       <c r="C50" s="58" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D50" s="0" t="n">
         <v>6</v>
@@ -21608,13 +21602,13 @@
     </row>
     <row r="51" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="146" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="B51" s="95" t="s">
         <v>1057</v>
       </c>
       <c r="C51" s="58" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>6</v>
@@ -21622,13 +21616,13 @@
     </row>
     <row r="52" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="59" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="B52" s="95" t="s">
         <v>1068</v>
       </c>
       <c r="C52" s="58" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D52" s="0" t="n">
         <v>6</v>
@@ -21636,13 +21630,13 @@
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="67" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="B53" s="99" t="s">
         <v>1077</v>
       </c>
       <c r="C53" s="66" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D53" s="69" t="n">
         <v>6</v>
@@ -21650,13 +21644,13 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="59" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="B54" s="59" t="s">
         <v>819</v>
       </c>
       <c r="C54" s="58" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="D54" s="0" t="n">
         <v>7</v>
@@ -21664,13 +21658,13 @@
     </row>
     <row r="55" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="59" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="B55" s="59" t="s">
         <v>828</v>
       </c>
       <c r="C55" s="58" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D55" s="0" t="n">
         <v>7</v>
@@ -21678,13 +21672,13 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="59" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="B56" s="59" t="s">
         <v>843</v>
       </c>
       <c r="C56" s="58" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D56" s="0" t="n">
         <v>7</v>
@@ -21692,13 +21686,13 @@
     </row>
     <row r="57" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="59" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="B57" s="59" t="s">
         <v>848</v>
       </c>
       <c r="C57" s="58" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D57" s="0" t="n">
         <v>7</v>
@@ -21706,13 +21700,13 @@
     </row>
     <row r="58" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="59" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="B58" s="59" t="s">
         <v>1088</v>
       </c>
       <c r="C58" s="58" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D58" s="0" t="n">
         <v>7</v>
@@ -21720,13 +21714,13 @@
     </row>
     <row r="59" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="67" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="B59" s="99" t="s">
         <v>1093</v>
       </c>
       <c r="C59" s="66" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D59" s="69" t="n">
         <v>7</v>
@@ -21734,13 +21728,13 @@
     </row>
     <row r="60" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="59" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="B60" s="59" t="s">
         <v>853</v>
       </c>
       <c r="C60" s="58" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D60" s="0" t="n">
         <v>8</v>
@@ -21748,13 +21742,13 @@
     </row>
     <row r="61" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="59" t="s">
-        <v>1652</v>
+        <v>1651</v>
       </c>
       <c r="B61" s="95" t="s">
         <v>868</v>
       </c>
       <c r="C61" s="58" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D61" s="0" t="n">
         <v>8</v>
@@ -21762,13 +21756,13 @@
     </row>
     <row r="62" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="59" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="B62" s="95" t="s">
         <v>873</v>
       </c>
       <c r="C62" s="58" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D62" s="0" t="n">
         <v>8</v>
@@ -21776,13 +21770,13 @@
     </row>
     <row r="63" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="59" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="B63" s="95" t="s">
         <v>880</v>
       </c>
       <c r="C63" s="58" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D63" s="0" t="n">
         <v>8</v>
@@ -21790,13 +21784,13 @@
     </row>
     <row r="64" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="59" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="B64" s="95" t="s">
         <v>887</v>
       </c>
       <c r="C64" s="58" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D64" s="0" t="n">
         <v>8</v>
@@ -21804,13 +21798,13 @@
     </row>
     <row r="65" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="59" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B65" s="59" t="s">
         <v>1106</v>
       </c>
       <c r="C65" s="58" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D65" s="0" t="n">
         <v>8</v>
@@ -21818,13 +21812,13 @@
     </row>
     <row r="66" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="59" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B66" s="95" t="s">
         <v>1117</v>
       </c>
       <c r="C66" s="58" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D66" s="0" t="n">
         <v>8</v>
@@ -21832,13 +21826,13 @@
     </row>
     <row r="67" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="67" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
       <c r="B67" s="99" t="s">
         <v>1120</v>
       </c>
       <c r="C67" s="66" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D67" s="69" t="n">
         <v>8</v>
@@ -21846,13 +21840,13 @@
     </row>
     <row r="68" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="59" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="B68" s="59" t="s">
         <v>898</v>
       </c>
       <c r="C68" s="58" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D68" s="0" t="n">
         <v>9</v>
@@ -21860,13 +21854,13 @@
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="59" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="B69" s="59" t="s">
         <v>905</v>
       </c>
       <c r="C69" s="58" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D69" s="0" t="n">
         <v>9</v>
@@ -21874,13 +21868,13 @@
     </row>
     <row r="70" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="59" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
       <c r="B70" s="95" t="s">
         <v>1127</v>
       </c>
       <c r="C70" s="58" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D70" s="0" t="n">
         <v>9</v>
@@ -21888,13 +21882,13 @@
     </row>
     <row r="71" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="59" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="B71" s="95" t="s">
         <v>1150</v>
       </c>
       <c r="C71" s="58" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D71" s="0" t="n">
         <v>9</v>
@@ -21902,13 +21896,13 @@
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="59" t="s">
-        <v>1663</v>
+        <v>1662</v>
       </c>
       <c r="B72" s="95" t="s">
         <v>1157</v>
       </c>
       <c r="C72" s="58" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D72" s="0" t="n">
         <v>9</v>
@@ -21916,22 +21910,275 @@
     </row>
     <row r="73" customFormat="false" ht="18.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="67" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="B73" s="99" t="s">
         <v>1164</v>
       </c>
       <c r="C73" s="66" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
       <c r="D73" s="69" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="146" t="s">
+        <v>1664</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C74" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="146" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C75" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="148" t="s">
+        <v>1666</v>
+      </c>
+      <c r="B76" s="69" t="s">
+        <v>1243</v>
+      </c>
+      <c r="C76" s="66" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D76" s="69" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="59" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C77" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="59" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B78" s="146" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C78" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="163" t="s">
+        <v>1669</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>1670</v>
+      </c>
+      <c r="C79" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D79" s="164" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="59" t="s">
+        <v>1671</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C80" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D80" s="164" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="67" t="s">
+        <v>1672</v>
+      </c>
+      <c r="B81" s="69" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C81" s="66" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D81" s="165" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="59" t="s">
+        <v>1673</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C82" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D82" s="164" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="59" t="s">
+        <v>1674</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>1361</v>
+      </c>
+      <c r="C83" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D83" s="164" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="59" t="s">
+        <v>1675</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>1365</v>
+      </c>
+      <c r="C84" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D84" s="164" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="59" t="s">
+        <v>1676</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C85" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="59" t="s">
+        <v>1677</v>
+      </c>
+      <c r="B86" s="0" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C86" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="67" t="s">
+        <v>1678</v>
+      </c>
+      <c r="B87" s="69" t="s">
+        <v>1449</v>
+      </c>
+      <c r="C87" s="66" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D87" s="69" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="59" t="s">
+        <v>1679</v>
+      </c>
+      <c r="B88" s="0" t="s">
+        <v>1462</v>
+      </c>
+      <c r="C88" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="59" t="s">
+        <v>1680</v>
+      </c>
+      <c r="B89" s="0" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C89" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="59" t="s">
+        <v>1681</v>
+      </c>
+      <c r="B90" s="0" t="s">
+        <v>1510</v>
+      </c>
+      <c r="C90" s="58" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="67" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B91" s="69" t="s">
+        <v>1547</v>
+      </c>
+      <c r="C91" s="66" t="s">
+        <v>1639</v>
+      </c>
+      <c r="D91" s="69" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>